<commit_message>
re-did fu18 with error
</commit_message>
<xml_diff>
--- a/data/update2019/ospree_2019update_dmb.xlsx
+++ b/data/update2019/ospree_2019update_dmb.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielbuonaiuto/Documents/git/ospree/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielbuonaiuto/Documents/git/ospree/data/update2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="460" windowWidth="25600" windowHeight="14240"/>
+    <workbookView xWindow="4440" yWindow="960" windowWidth="25600" windowHeight="15360" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="2" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="326">
   <si>
     <t>datasetID</t>
   </si>
@@ -1049,6 +1049,21 @@
   </si>
   <si>
     <t>ambient+5</t>
+  </si>
+  <si>
+    <t>adjmean</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>adjerror</t>
+  </si>
+  <si>
+    <t>3erro</t>
+  </si>
+  <si>
+    <t>unspecified</t>
   </si>
 </sst>
 </file>
@@ -1557,7 +1572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+    <sheetView topLeftCell="A63" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -3018,8 +3033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA30"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AC14" sqref="AC14"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2:AC30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3247,6 +3262,12 @@
       <c r="AB2">
         <v>4</v>
       </c>
+      <c r="AC2" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD2">
+        <v>3.8449999999999989</v>
+      </c>
       <c r="AE2" t="s">
         <v>306</v>
       </c>
@@ -3309,6 +3330,12 @@
       <c r="AB3">
         <v>4</v>
       </c>
+      <c r="AC3" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD3">
+        <v>3.0289999999999964</v>
+      </c>
       <c r="AE3" t="s">
         <v>306</v>
       </c>
@@ -3371,6 +3398,12 @@
       <c r="AB4">
         <v>4</v>
       </c>
+      <c r="AC4" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD4">
+        <v>2.7959999999999923</v>
+      </c>
       <c r="AE4" t="s">
         <v>306</v>
       </c>
@@ -3433,6 +3466,12 @@
       <c r="AB5">
         <v>4</v>
       </c>
+      <c r="AC5" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD5">
+        <v>2.9119999999999777</v>
+      </c>
       <c r="AE5" t="s">
         <v>306</v>
       </c>
@@ -3495,6 +3534,12 @@
       <c r="AB6">
         <v>4</v>
       </c>
+      <c r="AC6" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD6">
+        <v>2.4470000000000027</v>
+      </c>
       <c r="AE6" t="s">
         <v>306</v>
       </c>
@@ -3557,6 +3602,12 @@
       <c r="AB7">
         <v>4</v>
       </c>
+      <c r="AC7" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD7">
+        <v>2.6790000000000305</v>
+      </c>
       <c r="AE7" t="s">
         <v>306</v>
       </c>
@@ -3619,6 +3670,12 @@
       <c r="AB8">
         <v>4</v>
       </c>
+      <c r="AC8" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD8">
+        <v>6.9900000000000091</v>
+      </c>
       <c r="AE8" t="s">
         <v>306</v>
       </c>
@@ -3681,6 +3738,12 @@
       <c r="AB9">
         <v>4</v>
       </c>
+      <c r="AC9" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD9">
+        <v>1.7479999999999905</v>
+      </c>
       <c r="AE9" t="s">
         <v>306</v>
       </c>
@@ -3743,6 +3806,12 @@
       <c r="AB10">
         <v>4</v>
       </c>
+      <c r="AC10" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD10">
+        <v>3.8439999999999941</v>
+      </c>
       <c r="AE10" t="s">
         <v>306</v>
       </c>
@@ -3800,10 +3869,16 @@
         <v>1</v>
       </c>
       <c r="AA11">
-        <v>84.942000000000007</v>
+        <v>84.730000000000018</v>
       </c>
       <c r="AB11">
         <v>4</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD11">
+        <v>3.2409999999999854</v>
       </c>
       <c r="AE11" t="s">
         <v>306</v>
@@ -3862,10 +3937,16 @@
         <v>1</v>
       </c>
       <c r="AA12">
-        <v>84.942000000000007</v>
+        <v>84.730000000000018</v>
       </c>
       <c r="AB12">
         <v>4</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD12">
+        <v>4.1730000000000018</v>
       </c>
       <c r="AE12" t="s">
         <v>306</v>
@@ -3924,10 +4005,16 @@
         <v>1</v>
       </c>
       <c r="AA13">
-        <v>91.932000000000016</v>
+        <v>91.891999999999996</v>
       </c>
       <c r="AB13">
         <v>4</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD13">
+        <v>2.1370000000000005</v>
       </c>
       <c r="AE13" t="s">
         <v>306</v>
@@ -3986,10 +4073,16 @@
         <v>1</v>
       </c>
       <c r="AA14">
-        <v>92.980999999999995</v>
+        <v>92.831999999999994</v>
       </c>
       <c r="AB14">
         <v>4</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD14">
+        <v>3.2939999999999827</v>
       </c>
       <c r="AE14" t="s">
         <v>306</v>
@@ -4048,10 +4141,16 @@
         <v>1</v>
       </c>
       <c r="AA15">
-        <v>104.04899999999998</v>
+        <v>103.98599999999999</v>
       </c>
       <c r="AB15">
         <v>4</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD15">
+        <v>2.160000000000025</v>
       </c>
       <c r="AE15" t="s">
         <v>306</v>
@@ -4110,10 +4209,16 @@
         <v>1</v>
       </c>
       <c r="AA16">
-        <v>107.07799999999997</v>
+        <v>107.03899999999999</v>
       </c>
       <c r="AB16">
         <v>4</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD16">
+        <v>6.0970000000000368</v>
       </c>
       <c r="AE16" t="s">
         <v>306</v>
@@ -4172,10 +4277,16 @@
         <v>1</v>
       </c>
       <c r="AA17">
-        <v>106.96100000000001</v>
+        <v>107.03899999999999</v>
       </c>
       <c r="AB17">
         <v>4</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD17">
+        <v>6.0970000000000368</v>
       </c>
       <c r="AE17" t="s">
         <v>306</v>
@@ -4234,10 +4345,16 @@
         <v>1</v>
       </c>
       <c r="AA18">
-        <v>116.16500000000002</v>
+        <v>116.19799999999998</v>
       </c>
       <c r="AB18">
         <v>4</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD18">
+        <v>2.9960000000000377</v>
       </c>
       <c r="AE18" t="s">
         <v>306</v>
@@ -4301,6 +4418,12 @@
       <c r="AB19">
         <v>4</v>
       </c>
+      <c r="AC19" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD19">
+        <v>4.3930000000000007</v>
+      </c>
       <c r="AE19" t="s">
         <v>314</v>
       </c>
@@ -4363,6 +4486,12 @@
       <c r="AB20">
         <v>4</v>
       </c>
+      <c r="AC20" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD20">
+        <v>1.6350000000000193</v>
+      </c>
       <c r="AE20" t="s">
         <v>314</v>
       </c>
@@ -4425,6 +4554,12 @@
       <c r="AB21">
         <v>4</v>
       </c>
+      <c r="AC21" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD21">
+        <v>1.1479999999999961</v>
+      </c>
       <c r="AE21" t="s">
         <v>314</v>
       </c>
@@ -4487,6 +4622,12 @@
       <c r="AB22">
         <v>4</v>
       </c>
+      <c r="AC22" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD22">
+        <v>3.5459999999999923</v>
+      </c>
       <c r="AE22" t="s">
         <v>314</v>
       </c>
@@ -4549,6 +4690,12 @@
       <c r="AB23">
         <v>4</v>
       </c>
+      <c r="AC23" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD23">
+        <v>0.95900000000001739</v>
+      </c>
       <c r="AE23" t="s">
         <v>314</v>
       </c>
@@ -4611,6 +4758,12 @@
       <c r="AB24">
         <v>4</v>
       </c>
+      <c r="AC24" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD24">
+        <v>1.9510000000000076</v>
+      </c>
       <c r="AE24" t="s">
         <v>314</v>
       </c>
@@ -4673,6 +4826,12 @@
       <c r="AB25">
         <v>4</v>
       </c>
+      <c r="AC25" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD25">
+        <v>3.8379999999999939</v>
+      </c>
       <c r="AE25" t="s">
         <v>314</v>
       </c>
@@ -4735,6 +4894,12 @@
       <c r="AB26">
         <v>4</v>
       </c>
+      <c r="AC26" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD26">
+        <v>1.1929999999999978</v>
+      </c>
       <c r="AE26" t="s">
         <v>314</v>
       </c>
@@ -4797,6 +4962,12 @@
       <c r="AB27">
         <v>4</v>
       </c>
+      <c r="AC27" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD27">
+        <v>5.835000000000008</v>
+      </c>
       <c r="AE27" t="s">
         <v>314</v>
       </c>
@@ -4859,6 +5030,12 @@
       <c r="AB28">
         <v>4</v>
       </c>
+      <c r="AC28" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD28">
+        <v>5.2740000000000009</v>
+      </c>
       <c r="AE28" t="s">
         <v>314</v>
       </c>
@@ -4921,6 +5098,12 @@
       <c r="AB29">
         <v>4</v>
       </c>
+      <c r="AC29" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD29">
+        <v>5.7069999999999936</v>
+      </c>
       <c r="AE29" t="s">
         <v>314</v>
       </c>
@@ -4982,6 +5165,12 @@
       </c>
       <c r="AB30">
         <v>4</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD30">
+        <v>7.1979999999999933</v>
       </c>
       <c r="AE30" t="s">
         <v>314</v>
@@ -4999,25 +5188,25 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:T61"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7:N18"/>
+    <sheetView topLeftCell="E1" zoomScale="84" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7:T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
         <v>301</v>
       </c>
@@ -5030,8 +5219,14 @@
       <c r="I5" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J5" t="s">
+        <v>324</v>
+      </c>
+      <c r="K5" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="E6" t="s">
         <v>302</v>
       </c>
@@ -5045,14 +5240,21 @@
         <f>H6-228</f>
         <v>24</v>
       </c>
-      <c r="K6" t="s">
+      <c r="J6">
+        <v>255.845</v>
+      </c>
+      <c r="K6">
+        <f>J6-H6</f>
+        <v>3.8449999999999989</v>
+      </c>
+      <c r="O6" t="s">
         <v>309</v>
       </c>
-      <c r="L6" t="s">
+      <c r="P6" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
         <v>303</v>
       </c>
@@ -5066,20 +5268,34 @@
         <f t="shared" ref="I7:I14" si="0">H7-228</f>
         <v>22.835000000000008</v>
       </c>
-      <c r="K7" t="s">
+      <c r="J7">
+        <v>253.864</v>
+      </c>
+      <c r="K7">
+        <f t="shared" ref="K7:K14" si="1">J7-H7</f>
+        <v>3.0289999999999964</v>
+      </c>
+      <c r="O7" t="s">
         <v>315</v>
       </c>
-      <c r="L7">
+      <c r="P7">
         <v>0</v>
       </c>
-      <c r="M7">
+      <c r="Q7">
         <v>0.22800000000000001</v>
       </c>
-      <c r="N7">
+      <c r="R7">
         <v>130.97200000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S7">
+        <v>135.36500000000001</v>
+      </c>
+      <c r="T7">
+        <f>S7-R7</f>
+        <v>4.3930000000000007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="G8">
         <v>-0.60599999999999998</v>
       </c>
@@ -5090,20 +5306,34 @@
         <f t="shared" si="0"/>
         <v>30.990000000000009</v>
       </c>
-      <c r="K8" t="s">
+      <c r="J8">
+        <v>261.786</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>2.7959999999999923</v>
+      </c>
+      <c r="O8" t="s">
         <v>316</v>
       </c>
-      <c r="L8">
+      <c r="P8">
         <v>0</v>
       </c>
-      <c r="M8">
+      <c r="Q8">
         <v>0.39</v>
       </c>
-      <c r="N8">
+      <c r="R8">
         <v>130.27799999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S8">
+        <v>131.91300000000001</v>
+      </c>
+      <c r="T8">
+        <f t="shared" ref="T8:T18" si="2">S8-R8</f>
+        <v>1.6350000000000193</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="G9">
         <v>-0.105</v>
       </c>
@@ -5114,17 +5344,31 @@
         <f t="shared" si="0"/>
         <v>32.971000000000004</v>
       </c>
-      <c r="L9">
+      <c r="J9">
+        <v>263.88299999999998</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>2.9119999999999777</v>
+      </c>
+      <c r="P9">
         <v>1</v>
       </c>
-      <c r="M9">
+      <c r="Q9">
         <v>1.2010000000000001</v>
       </c>
-      <c r="N9">
+      <c r="R9">
         <v>129.38499999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S9">
+        <v>130.53299999999999</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="2"/>
+        <v>1.1479999999999961</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="G10">
         <v>-4.0000000000000001E-3</v>
       </c>
@@ -5135,17 +5379,31 @@
         <f t="shared" si="0"/>
         <v>35.882999999999981</v>
       </c>
-      <c r="L10">
+      <c r="J10">
+        <v>266.33</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>2.4470000000000027</v>
+      </c>
+      <c r="P10">
         <v>2</v>
       </c>
-      <c r="M10">
+      <c r="Q10">
         <v>1.83</v>
       </c>
-      <c r="N10">
+      <c r="R10">
         <v>123.929</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S10">
+        <v>127.47499999999999</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="2"/>
+        <v>3.5459999999999923</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="G11">
         <v>-4.0000000000000001E-3</v>
       </c>
@@ -5156,17 +5414,31 @@
         <f t="shared" si="0"/>
         <v>40.077999999999975</v>
       </c>
-      <c r="L11">
+      <c r="J11">
+        <v>270.75700000000001</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>2.6790000000000305</v>
+      </c>
+      <c r="P11">
         <v>2</v>
       </c>
-      <c r="M11">
+      <c r="Q11">
         <v>2.0840000000000001</v>
       </c>
-      <c r="N11">
+      <c r="R11">
         <v>127.996</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S11">
+        <v>128.95500000000001</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="2"/>
+        <v>0.95900000000001739</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="G12">
         <v>0.58699999999999997</v>
       </c>
@@ -5177,17 +5449,31 @@
         <f t="shared" si="0"/>
         <v>41.009999999999991</v>
       </c>
-      <c r="L12">
+      <c r="J12">
+        <v>276</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>6.9900000000000091</v>
+      </c>
+      <c r="P12">
         <v>2</v>
       </c>
-      <c r="M12">
+      <c r="Q12">
         <v>2.2360000000000002</v>
       </c>
-      <c r="N12">
+      <c r="R12">
         <v>127.004</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S12">
+        <v>128.95500000000001</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="2"/>
+        <v>1.9510000000000076</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="G13">
         <v>0.68799999999999994</v>
       </c>
@@ -5198,17 +5484,31 @@
         <f t="shared" si="0"/>
         <v>45.086999999999989</v>
       </c>
-      <c r="L13">
+      <c r="J13">
+        <v>274.83499999999998</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>1.7479999999999905</v>
+      </c>
+      <c r="P13">
         <v>3</v>
       </c>
-      <c r="M13">
+      <c r="Q13">
         <v>2.6619999999999999</v>
       </c>
-      <c r="N13">
+      <c r="R13">
         <v>124.821</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S13">
+        <v>128.65899999999999</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="2"/>
+        <v>3.8379999999999939</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="G14">
         <v>1.59</v>
       </c>
@@ -5219,66 +5519,108 @@
         <f t="shared" si="0"/>
         <v>44.038999999999987</v>
       </c>
-      <c r="L14">
+      <c r="J14">
+        <v>275.88299999999998</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999941</v>
+      </c>
+      <c r="P14">
         <v>4</v>
       </c>
-      <c r="M14">
+      <c r="Q14">
         <v>3.6259999999999999</v>
       </c>
-      <c r="N14">
+      <c r="R14">
         <v>121.64700000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="L15">
+      <c r="S14">
+        <v>122.84</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="2"/>
+        <v>1.1929999999999978</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="P15">
         <v>4</v>
       </c>
-      <c r="M15">
+      <c r="Q15">
         <v>3.7480000000000002</v>
       </c>
-      <c r="N15">
+      <c r="R15">
         <v>120.556</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="L16">
+      <c r="S15">
+        <v>126.39100000000001</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="2"/>
+        <v>5.835000000000008</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="P16">
         <v>4</v>
       </c>
-      <c r="M16">
+      <c r="Q16">
         <v>4.0519999999999996</v>
       </c>
-      <c r="N16">
+      <c r="R16">
         <v>115.39700000000001</v>
       </c>
-    </row>
-    <row r="17" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="L17">
+      <c r="S16">
+        <v>120.67100000000001</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="2"/>
+        <v>5.2740000000000009</v>
+      </c>
+    </row>
+    <row r="17" spans="5:20" x14ac:dyDescent="0.2">
+      <c r="P17">
         <v>5</v>
       </c>
-      <c r="M17">
+      <c r="Q17">
         <v>4.8639999999999999</v>
       </c>
-      <c r="N17">
+      <c r="R17">
         <v>108.849</v>
       </c>
-    </row>
-    <row r="18" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="L18">
+      <c r="S17">
+        <v>114.556</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="2"/>
+        <v>5.7069999999999936</v>
+      </c>
+    </row>
+    <row r="18" spans="5:20" x14ac:dyDescent="0.2">
+      <c r="P18">
         <v>5</v>
       </c>
-      <c r="M18">
+      <c r="Q18">
         <v>5.3609999999999998</v>
       </c>
-      <c r="N18">
+      <c r="R18">
         <v>106.76600000000001</v>
       </c>
-    </row>
-    <row r="19" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="S18">
+        <v>113.964</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="2"/>
+        <v>7.1979999999999933</v>
+      </c>
+    </row>
+    <row r="19" spans="5:20" x14ac:dyDescent="0.2">
       <c r="E19" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="20" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="5:20" x14ac:dyDescent="0.2">
       <c r="E20" t="s">
         <v>302</v>
       </c>
@@ -5288,8 +5630,17 @@
       <c r="H20" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="21" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="I20" t="s">
+        <v>321</v>
+      </c>
+      <c r="J20" t="s">
+        <v>322</v>
+      </c>
+      <c r="K20" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="21" spans="5:20" x14ac:dyDescent="0.2">
       <c r="E21" t="s">
         <v>310</v>
       </c>
@@ -5297,119 +5648,832 @@
         <v>311</v>
       </c>
       <c r="G21">
-        <v>-4.0000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="H21">
-        <v>257.94200000000001</v>
+        <v>257.73</v>
       </c>
       <c r="I21">
         <f>H21-173</f>
-        <v>84.942000000000007</v>
-      </c>
-    </row>
-    <row r="22" spans="5:14" x14ac:dyDescent="0.2">
+        <v>84.730000000000018</v>
+      </c>
+      <c r="J21">
+        <v>260.971</v>
+      </c>
+      <c r="K21">
+        <f>J21-H21</f>
+        <v>3.2409999999999854</v>
+      </c>
+    </row>
+    <row r="22" spans="5:20" x14ac:dyDescent="0.2">
       <c r="F22" t="s">
         <v>311</v>
       </c>
       <c r="G22">
-        <v>8.5999999999999993E-2</v>
+        <v>0.105</v>
       </c>
       <c r="H22">
-        <v>257.94200000000001</v>
+        <v>257.73</v>
       </c>
       <c r="I22">
-        <f t="shared" ref="I22:I28" si="1">H22-173</f>
-        <v>84.942000000000007</v>
-      </c>
-    </row>
-    <row r="23" spans="5:14" x14ac:dyDescent="0.2">
+        <f t="shared" ref="I22:I28" si="3">H22-173</f>
+        <v>84.730000000000018</v>
+      </c>
+      <c r="J22">
+        <v>261.90300000000002</v>
+      </c>
+      <c r="K22">
+        <f t="shared" ref="K22:K28" si="4">J22-H22</f>
+        <v>4.1730000000000018</v>
+      </c>
+    </row>
+    <row r="23" spans="5:20" x14ac:dyDescent="0.2">
       <c r="F23">
         <v>1</v>
       </c>
       <c r="G23">
-        <v>0.98899999999999999</v>
+        <v>1.0009999999999999</v>
       </c>
       <c r="H23">
-        <v>264.93200000000002</v>
+        <v>264.892</v>
       </c>
       <c r="I23">
-        <f t="shared" si="1"/>
-        <v>91.932000000000016</v>
-      </c>
-    </row>
-    <row r="24" spans="5:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>91.891999999999996</v>
+      </c>
+      <c r="J23">
+        <v>267.029</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="4"/>
+        <v>2.1370000000000005</v>
+      </c>
+    </row>
+    <row r="24" spans="5:20" x14ac:dyDescent="0.2">
       <c r="F24">
         <v>1</v>
       </c>
       <c r="G24">
-        <v>1.1890000000000001</v>
+        <v>1.2030000000000001</v>
       </c>
       <c r="H24">
-        <v>265.98099999999999</v>
+        <v>265.83199999999999</v>
       </c>
       <c r="I24">
-        <f t="shared" si="1"/>
-        <v>92.980999999999995</v>
-      </c>
-    </row>
-    <row r="25" spans="5:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>92.831999999999994</v>
+      </c>
+      <c r="J24">
+        <v>269.12599999999998</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="4"/>
+        <v>3.2939999999999827</v>
+      </c>
+    </row>
+    <row r="25" spans="5:20" x14ac:dyDescent="0.2">
       <c r="F25">
         <v>1</v>
       </c>
       <c r="G25">
-        <v>1.089</v>
+        <v>1.1020000000000001</v>
       </c>
       <c r="H25">
-        <v>277.04899999999998</v>
+        <v>276.98599999999999</v>
       </c>
       <c r="I25">
-        <f t="shared" si="1"/>
-        <v>104.04899999999998</v>
-      </c>
-    </row>
-    <row r="26" spans="5:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>103.98599999999999</v>
+      </c>
+      <c r="J25">
+        <v>279.14600000000002</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="4"/>
+        <v>2.160000000000025</v>
+      </c>
+    </row>
+    <row r="26" spans="5:20" x14ac:dyDescent="0.2">
       <c r="F26">
         <v>3</v>
       </c>
       <c r="G26">
-        <v>2.4830000000000001</v>
+        <v>2.512</v>
       </c>
       <c r="H26">
-        <v>280.07799999999997</v>
+        <v>280.03899999999999</v>
       </c>
       <c r="I26">
-        <f t="shared" si="1"/>
-        <v>107.07799999999997</v>
-      </c>
-    </row>
-    <row r="27" spans="5:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>107.03899999999999</v>
+      </c>
+      <c r="J26">
+        <v>286.13600000000002</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="4"/>
+        <v>6.0970000000000368</v>
+      </c>
+    </row>
+    <row r="27" spans="5:20" x14ac:dyDescent="0.2">
       <c r="F27">
         <v>3</v>
       </c>
       <c r="G27">
-        <v>2.984</v>
+        <v>3.0059999999999998</v>
       </c>
       <c r="H27">
-        <v>279.96100000000001</v>
+        <v>280.03899999999999</v>
       </c>
       <c r="I27">
-        <f t="shared" si="1"/>
-        <v>106.96100000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="5:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>107.03899999999999</v>
+      </c>
+      <c r="J27">
+        <v>286.13600000000002</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="4"/>
+        <v>6.0970000000000368</v>
+      </c>
+    </row>
+    <row r="28" spans="5:20" x14ac:dyDescent="0.2">
       <c r="F28">
         <v>4</v>
       </c>
       <c r="G28">
-        <v>4.3780000000000001</v>
+        <v>4.4160000000000004</v>
       </c>
       <c r="H28">
-        <v>289.16500000000002</v>
+        <v>289.19799999999998</v>
       </c>
       <c r="I28">
-        <f t="shared" si="1"/>
-        <v>116.16500000000002</v>
+        <f t="shared" si="3"/>
+        <v>116.19799999999998</v>
+      </c>
+      <c r="J28">
+        <v>292.19400000000002</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="4"/>
+        <v>2.9960000000000377</v>
+      </c>
+    </row>
+    <row r="32" spans="5:20" x14ac:dyDescent="0.2">
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <v>20</v>
+      </c>
+      <c r="P32">
+        <v>20</v>
+      </c>
+      <c r="Q32">
+        <v>20</v>
+      </c>
+      <c r="R32">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+      <c r="S32">
+        <v>260.971</v>
+      </c>
+    </row>
+    <row r="33" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="M33">
+        <v>2</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <v>194</v>
+      </c>
+      <c r="P33">
+        <v>194</v>
+      </c>
+      <c r="Q33">
+        <v>194</v>
+      </c>
+      <c r="R33">
+        <v>0.115</v>
+      </c>
+      <c r="S33">
+        <v>261.90300000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="M34">
+        <v>3</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <v>171</v>
+      </c>
+      <c r="P34">
+        <v>171</v>
+      </c>
+      <c r="Q34">
+        <v>171</v>
+      </c>
+      <c r="R34">
+        <v>1.012</v>
+      </c>
+      <c r="S34">
+        <v>267.029</v>
+      </c>
+    </row>
+    <row r="35" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>76</v>
+      </c>
+      <c r="F35">
+        <v>76</v>
+      </c>
+      <c r="G35">
+        <v>76</v>
+      </c>
+      <c r="H35">
+        <v>-1.6990000000000001</v>
+      </c>
+      <c r="I35">
+        <v>255.845</v>
+      </c>
+      <c r="M35">
+        <v>4</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <v>109</v>
+      </c>
+      <c r="P35">
+        <v>109</v>
+      </c>
+      <c r="Q35">
+        <v>109</v>
+      </c>
+      <c r="R35">
+        <v>1.2230000000000001</v>
+      </c>
+      <c r="S35">
+        <v>269.12599999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>94</v>
+      </c>
+      <c r="F36">
+        <v>94</v>
+      </c>
+      <c r="G36">
+        <v>94</v>
+      </c>
+      <c r="H36">
+        <v>-1.4990000000000001</v>
+      </c>
+      <c r="I36">
+        <v>253.864</v>
+      </c>
+      <c r="M36">
+        <v>5</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <v>77</v>
+      </c>
+      <c r="P36">
+        <v>77</v>
+      </c>
+      <c r="Q36">
+        <v>77</v>
+      </c>
+      <c r="R36">
+        <v>1.1020000000000001</v>
+      </c>
+      <c r="S36">
+        <v>279.14600000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>92</v>
+      </c>
+      <c r="F37">
+        <v>92</v>
+      </c>
+      <c r="G37">
+        <v>92</v>
+      </c>
+      <c r="H37">
+        <v>-0.59599999999999997</v>
+      </c>
+      <c r="I37">
+        <v>261.786</v>
+      </c>
+      <c r="M37">
+        <v>6</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <v>71</v>
+      </c>
+      <c r="P37">
+        <v>71</v>
+      </c>
+      <c r="Q37">
+        <v>71</v>
+      </c>
+      <c r="R37">
+        <v>2.512</v>
+      </c>
+      <c r="S37">
+        <v>286.13600000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C38">
+        <v>4</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>93</v>
+      </c>
+      <c r="F38">
+        <v>93</v>
+      </c>
+      <c r="G38">
+        <v>93</v>
+      </c>
+      <c r="H38">
+        <v>-0.115</v>
+      </c>
+      <c r="I38">
+        <v>263.88299999999998</v>
+      </c>
+      <c r="M38">
+        <v>7</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <v>124</v>
+      </c>
+      <c r="P38">
+        <v>124</v>
+      </c>
+      <c r="Q38">
+        <v>124</v>
+      </c>
+      <c r="R38">
+        <v>2.996</v>
+      </c>
+      <c r="S38">
+        <v>286.13600000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C39">
+        <v>5</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>169</v>
+      </c>
+      <c r="F39">
+        <v>169</v>
+      </c>
+      <c r="G39">
+        <v>169</v>
+      </c>
+      <c r="H39">
+        <v>1.6E-2</v>
+      </c>
+      <c r="I39">
+        <v>266.33</v>
+      </c>
+      <c r="M39">
+        <v>8</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <v>92</v>
+      </c>
+      <c r="P39">
+        <v>92</v>
+      </c>
+      <c r="Q39">
+        <v>92</v>
+      </c>
+      <c r="R39">
+        <v>4.4260000000000002</v>
+      </c>
+      <c r="S39">
+        <v>292.19400000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C40">
+        <v>6</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>140</v>
+      </c>
+      <c r="F40">
+        <v>140</v>
+      </c>
+      <c r="G40">
+        <v>140</v>
+      </c>
+      <c r="H40">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="I40">
+        <v>270.75700000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C41">
+        <v>7</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>141</v>
+      </c>
+      <c r="F41">
+        <v>141</v>
+      </c>
+      <c r="G41">
+        <v>141</v>
+      </c>
+      <c r="H41">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="I41">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="42" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C42">
+        <v>8</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>72</v>
+      </c>
+      <c r="F42">
+        <v>72</v>
+      </c>
+      <c r="G42">
+        <v>72</v>
+      </c>
+      <c r="H42">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="I42">
+        <v>274.83499999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C43">
+        <v>9</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>23</v>
+      </c>
+      <c r="F43">
+        <v>23</v>
+      </c>
+      <c r="G43">
+        <v>23</v>
+      </c>
+      <c r="H43">
+        <v>1.6</v>
+      </c>
+      <c r="I43">
+        <v>275.88299999999998</v>
+      </c>
+    </row>
+    <row r="50" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="L50">
+        <v>2</v>
+      </c>
+      <c r="M50">
+        <v>0</v>
+      </c>
+      <c r="N50">
+        <v>94</v>
+      </c>
+      <c r="O50">
+        <v>94</v>
+      </c>
+      <c r="P50">
+        <v>94</v>
+      </c>
+      <c r="Q50">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="R50">
+        <v>135.36500000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="L51">
+        <v>3</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+      <c r="N51">
+        <v>89</v>
+      </c>
+      <c r="O51">
+        <v>89</v>
+      </c>
+      <c r="P51">
+        <v>89</v>
+      </c>
+      <c r="Q51">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="R51">
+        <v>131.91300000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="L52">
+        <v>4</v>
+      </c>
+      <c r="M52">
+        <v>0</v>
+      </c>
+      <c r="N52">
+        <v>100</v>
+      </c>
+      <c r="O52">
+        <v>100</v>
+      </c>
+      <c r="P52">
+        <v>100</v>
+      </c>
+      <c r="Q52">
+        <v>1.1819999999999999</v>
+      </c>
+      <c r="R52">
+        <v>130.53299999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="L53">
+        <v>5</v>
+      </c>
+      <c r="M53">
+        <v>0</v>
+      </c>
+      <c r="N53">
+        <v>153</v>
+      </c>
+      <c r="O53">
+        <v>153</v>
+      </c>
+      <c r="P53">
+        <v>153</v>
+      </c>
+      <c r="Q53">
+        <v>1.8080000000000001</v>
+      </c>
+      <c r="R53">
+        <v>127.47499999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="L54">
+        <v>6</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54">
+        <v>164</v>
+      </c>
+      <c r="O54">
+        <v>164</v>
+      </c>
+      <c r="P54">
+        <v>164</v>
+      </c>
+      <c r="Q54">
+        <v>2.0609999999999999</v>
+      </c>
+      <c r="R54">
+        <v>128.95500000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="L55">
+        <v>7</v>
+      </c>
+      <c r="M55">
+        <v>0</v>
+      </c>
+      <c r="N55">
+        <v>95</v>
+      </c>
+      <c r="O55">
+        <v>95</v>
+      </c>
+      <c r="P55">
+        <v>95</v>
+      </c>
+      <c r="Q55">
+        <v>2.222</v>
+      </c>
+      <c r="R55">
+        <v>128.95500000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="L56">
+        <v>8</v>
+      </c>
+      <c r="M56">
+        <v>0</v>
+      </c>
+      <c r="N56">
+        <v>43</v>
+      </c>
+      <c r="O56">
+        <v>43</v>
+      </c>
+      <c r="P56">
+        <v>43</v>
+      </c>
+      <c r="Q56">
+        <v>2.6459999999999999</v>
+      </c>
+      <c r="R56">
+        <v>128.65899999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="L57">
+        <v>9</v>
+      </c>
+      <c r="M57">
+        <v>0</v>
+      </c>
+      <c r="N57">
+        <v>83</v>
+      </c>
+      <c r="O57">
+        <v>83</v>
+      </c>
+      <c r="P57">
+        <v>83</v>
+      </c>
+      <c r="Q57">
+        <v>3.6059999999999999</v>
+      </c>
+      <c r="R57">
+        <v>122.84</v>
+      </c>
+    </row>
+    <row r="58" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="L58">
+        <v>10</v>
+      </c>
+      <c r="M58">
+        <v>0</v>
+      </c>
+      <c r="N58">
+        <v>122</v>
+      </c>
+      <c r="O58">
+        <v>122</v>
+      </c>
+      <c r="P58">
+        <v>122</v>
+      </c>
+      <c r="Q58">
+        <v>3.7370000000000001</v>
+      </c>
+      <c r="R58">
+        <v>126.39100000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="L59">
+        <v>11</v>
+      </c>
+      <c r="M59">
+        <v>0</v>
+      </c>
+      <c r="N59">
+        <v>119</v>
+      </c>
+      <c r="O59">
+        <v>119</v>
+      </c>
+      <c r="P59">
+        <v>119</v>
+      </c>
+      <c r="Q59">
+        <v>4.03</v>
+      </c>
+      <c r="R59">
+        <v>120.67100000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="L60">
+        <v>12</v>
+      </c>
+      <c r="M60">
+        <v>0</v>
+      </c>
+      <c r="N60">
+        <v>56</v>
+      </c>
+      <c r="O60">
+        <v>56</v>
+      </c>
+      <c r="P60">
+        <v>56</v>
+      </c>
+      <c r="Q60">
+        <v>4.8380000000000001</v>
+      </c>
+      <c r="R60">
+        <v>114.556</v>
+      </c>
+    </row>
+    <row r="61" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="L61">
+        <v>13</v>
+      </c>
+      <c r="M61">
+        <v>0</v>
+      </c>
+      <c r="N61">
+        <v>68</v>
+      </c>
+      <c r="O61">
+        <v>68</v>
+      </c>
+      <c r="P61">
+        <v>68</v>
+      </c>
+      <c r="Q61">
+        <v>5.343</v>
+      </c>
+      <c r="R61">
+        <v>113.964</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding back in Dan's file
Sorry!
</commit_message>
<xml_diff>
--- a/data/update2019/ospree_2019update_dmb.xlsx
+++ b/data/update2019/ospree_2019update_dmb.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielbuonaiuto/Documents/git/ospree/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielbuonaiuto/Documents/git/ospree/data/update2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="460" windowWidth="25600" windowHeight="14240"/>
+    <workbookView xWindow="4440" yWindow="960" windowWidth="25600" windowHeight="15360" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="2" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="326">
   <si>
     <t>datasetID</t>
   </si>
@@ -1049,6 +1049,21 @@
   </si>
   <si>
     <t>ambient+5</t>
+  </si>
+  <si>
+    <t>adjmean</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>adjerror</t>
+  </si>
+  <si>
+    <t>3erro</t>
+  </si>
+  <si>
+    <t>unspecified</t>
   </si>
 </sst>
 </file>
@@ -1557,7 +1572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+    <sheetView topLeftCell="A63" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -3018,8 +3033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA30"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AC14" sqref="AC14"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2:AC30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3247,6 +3262,12 @@
       <c r="AB2">
         <v>4</v>
       </c>
+      <c r="AC2" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD2">
+        <v>3.8449999999999989</v>
+      </c>
       <c r="AE2" t="s">
         <v>306</v>
       </c>
@@ -3309,6 +3330,12 @@
       <c r="AB3">
         <v>4</v>
       </c>
+      <c r="AC3" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD3">
+        <v>3.0289999999999964</v>
+      </c>
       <c r="AE3" t="s">
         <v>306</v>
       </c>
@@ -3371,6 +3398,12 @@
       <c r="AB4">
         <v>4</v>
       </c>
+      <c r="AC4" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD4">
+        <v>2.7959999999999923</v>
+      </c>
       <c r="AE4" t="s">
         <v>306</v>
       </c>
@@ -3433,6 +3466,12 @@
       <c r="AB5">
         <v>4</v>
       </c>
+      <c r="AC5" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD5">
+        <v>2.9119999999999777</v>
+      </c>
       <c r="AE5" t="s">
         <v>306</v>
       </c>
@@ -3495,6 +3534,12 @@
       <c r="AB6">
         <v>4</v>
       </c>
+      <c r="AC6" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD6">
+        <v>2.4470000000000027</v>
+      </c>
       <c r="AE6" t="s">
         <v>306</v>
       </c>
@@ -3557,6 +3602,12 @@
       <c r="AB7">
         <v>4</v>
       </c>
+      <c r="AC7" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD7">
+        <v>2.6790000000000305</v>
+      </c>
       <c r="AE7" t="s">
         <v>306</v>
       </c>
@@ -3619,6 +3670,12 @@
       <c r="AB8">
         <v>4</v>
       </c>
+      <c r="AC8" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD8">
+        <v>6.9900000000000091</v>
+      </c>
       <c r="AE8" t="s">
         <v>306</v>
       </c>
@@ -3681,6 +3738,12 @@
       <c r="AB9">
         <v>4</v>
       </c>
+      <c r="AC9" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD9">
+        <v>1.7479999999999905</v>
+      </c>
       <c r="AE9" t="s">
         <v>306</v>
       </c>
@@ -3743,6 +3806,12 @@
       <c r="AB10">
         <v>4</v>
       </c>
+      <c r="AC10" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD10">
+        <v>3.8439999999999941</v>
+      </c>
       <c r="AE10" t="s">
         <v>306</v>
       </c>
@@ -3800,10 +3869,16 @@
         <v>1</v>
       </c>
       <c r="AA11">
-        <v>84.942000000000007</v>
+        <v>84.730000000000018</v>
       </c>
       <c r="AB11">
         <v>4</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD11">
+        <v>3.2409999999999854</v>
       </c>
       <c r="AE11" t="s">
         <v>306</v>
@@ -3862,10 +3937,16 @@
         <v>1</v>
       </c>
       <c r="AA12">
-        <v>84.942000000000007</v>
+        <v>84.730000000000018</v>
       </c>
       <c r="AB12">
         <v>4</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD12">
+        <v>4.1730000000000018</v>
       </c>
       <c r="AE12" t="s">
         <v>306</v>
@@ -3924,10 +4005,16 @@
         <v>1</v>
       </c>
       <c r="AA13">
-        <v>91.932000000000016</v>
+        <v>91.891999999999996</v>
       </c>
       <c r="AB13">
         <v>4</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD13">
+        <v>2.1370000000000005</v>
       </c>
       <c r="AE13" t="s">
         <v>306</v>
@@ -3986,10 +4073,16 @@
         <v>1</v>
       </c>
       <c r="AA14">
-        <v>92.980999999999995</v>
+        <v>92.831999999999994</v>
       </c>
       <c r="AB14">
         <v>4</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD14">
+        <v>3.2939999999999827</v>
       </c>
       <c r="AE14" t="s">
         <v>306</v>
@@ -4048,10 +4141,16 @@
         <v>1</v>
       </c>
       <c r="AA15">
-        <v>104.04899999999998</v>
+        <v>103.98599999999999</v>
       </c>
       <c r="AB15">
         <v>4</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD15">
+        <v>2.160000000000025</v>
       </c>
       <c r="AE15" t="s">
         <v>306</v>
@@ -4110,10 +4209,16 @@
         <v>1</v>
       </c>
       <c r="AA16">
-        <v>107.07799999999997</v>
+        <v>107.03899999999999</v>
       </c>
       <c r="AB16">
         <v>4</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD16">
+        <v>6.0970000000000368</v>
       </c>
       <c r="AE16" t="s">
         <v>306</v>
@@ -4172,10 +4277,16 @@
         <v>1</v>
       </c>
       <c r="AA17">
-        <v>106.96100000000001</v>
+        <v>107.03899999999999</v>
       </c>
       <c r="AB17">
         <v>4</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD17">
+        <v>6.0970000000000368</v>
       </c>
       <c r="AE17" t="s">
         <v>306</v>
@@ -4234,10 +4345,16 @@
         <v>1</v>
       </c>
       <c r="AA18">
-        <v>116.16500000000002</v>
+        <v>116.19799999999998</v>
       </c>
       <c r="AB18">
         <v>4</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD18">
+        <v>2.9960000000000377</v>
       </c>
       <c r="AE18" t="s">
         <v>306</v>
@@ -4301,6 +4418,12 @@
       <c r="AB19">
         <v>4</v>
       </c>
+      <c r="AC19" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD19">
+        <v>4.3930000000000007</v>
+      </c>
       <c r="AE19" t="s">
         <v>314</v>
       </c>
@@ -4363,6 +4486,12 @@
       <c r="AB20">
         <v>4</v>
       </c>
+      <c r="AC20" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD20">
+        <v>1.6350000000000193</v>
+      </c>
       <c r="AE20" t="s">
         <v>314</v>
       </c>
@@ -4425,6 +4554,12 @@
       <c r="AB21">
         <v>4</v>
       </c>
+      <c r="AC21" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD21">
+        <v>1.1479999999999961</v>
+      </c>
       <c r="AE21" t="s">
         <v>314</v>
       </c>
@@ -4487,6 +4622,12 @@
       <c r="AB22">
         <v>4</v>
       </c>
+      <c r="AC22" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD22">
+        <v>3.5459999999999923</v>
+      </c>
       <c r="AE22" t="s">
         <v>314</v>
       </c>
@@ -4549,6 +4690,12 @@
       <c r="AB23">
         <v>4</v>
       </c>
+      <c r="AC23" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD23">
+        <v>0.95900000000001739</v>
+      </c>
       <c r="AE23" t="s">
         <v>314</v>
       </c>
@@ -4611,6 +4758,12 @@
       <c r="AB24">
         <v>4</v>
       </c>
+      <c r="AC24" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD24">
+        <v>1.9510000000000076</v>
+      </c>
       <c r="AE24" t="s">
         <v>314</v>
       </c>
@@ -4673,6 +4826,12 @@
       <c r="AB25">
         <v>4</v>
       </c>
+      <c r="AC25" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD25">
+        <v>3.8379999999999939</v>
+      </c>
       <c r="AE25" t="s">
         <v>314</v>
       </c>
@@ -4735,6 +4894,12 @@
       <c r="AB26">
         <v>4</v>
       </c>
+      <c r="AC26" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD26">
+        <v>1.1929999999999978</v>
+      </c>
       <c r="AE26" t="s">
         <v>314</v>
       </c>
@@ -4797,6 +4962,12 @@
       <c r="AB27">
         <v>4</v>
       </c>
+      <c r="AC27" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD27">
+        <v>5.835000000000008</v>
+      </c>
       <c r="AE27" t="s">
         <v>314</v>
       </c>
@@ -4859,6 +5030,12 @@
       <c r="AB28">
         <v>4</v>
       </c>
+      <c r="AC28" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD28">
+        <v>5.2740000000000009</v>
+      </c>
       <c r="AE28" t="s">
         <v>314</v>
       </c>
@@ -4921,6 +5098,12 @@
       <c r="AB29">
         <v>4</v>
       </c>
+      <c r="AC29" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD29">
+        <v>5.7069999999999936</v>
+      </c>
       <c r="AE29" t="s">
         <v>314</v>
       </c>
@@ -4982,6 +5165,12 @@
       </c>
       <c r="AB30">
         <v>4</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD30">
+        <v>7.1979999999999933</v>
       </c>
       <c r="AE30" t="s">
         <v>314</v>
@@ -4999,25 +5188,25 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:T61"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7:N18"/>
+    <sheetView topLeftCell="E1" zoomScale="84" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7:T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
         <v>301</v>
       </c>
@@ -5030,8 +5219,14 @@
       <c r="I5" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J5" t="s">
+        <v>324</v>
+      </c>
+      <c r="K5" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="E6" t="s">
         <v>302</v>
       </c>
@@ -5045,14 +5240,21 @@
         <f>H6-228</f>
         <v>24</v>
       </c>
-      <c r="K6" t="s">
+      <c r="J6">
+        <v>255.845</v>
+      </c>
+      <c r="K6">
+        <f>J6-H6</f>
+        <v>3.8449999999999989</v>
+      </c>
+      <c r="O6" t="s">
         <v>309</v>
       </c>
-      <c r="L6" t="s">
+      <c r="P6" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
         <v>303</v>
       </c>
@@ -5066,20 +5268,34 @@
         <f t="shared" ref="I7:I14" si="0">H7-228</f>
         <v>22.835000000000008</v>
       </c>
-      <c r="K7" t="s">
+      <c r="J7">
+        <v>253.864</v>
+      </c>
+      <c r="K7">
+        <f t="shared" ref="K7:K14" si="1">J7-H7</f>
+        <v>3.0289999999999964</v>
+      </c>
+      <c r="O7" t="s">
         <v>315</v>
       </c>
-      <c r="L7">
+      <c r="P7">
         <v>0</v>
       </c>
-      <c r="M7">
+      <c r="Q7">
         <v>0.22800000000000001</v>
       </c>
-      <c r="N7">
+      <c r="R7">
         <v>130.97200000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S7">
+        <v>135.36500000000001</v>
+      </c>
+      <c r="T7">
+        <f>S7-R7</f>
+        <v>4.3930000000000007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="G8">
         <v>-0.60599999999999998</v>
       </c>
@@ -5090,20 +5306,34 @@
         <f t="shared" si="0"/>
         <v>30.990000000000009</v>
       </c>
-      <c r="K8" t="s">
+      <c r="J8">
+        <v>261.786</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>2.7959999999999923</v>
+      </c>
+      <c r="O8" t="s">
         <v>316</v>
       </c>
-      <c r="L8">
+      <c r="P8">
         <v>0</v>
       </c>
-      <c r="M8">
+      <c r="Q8">
         <v>0.39</v>
       </c>
-      <c r="N8">
+      <c r="R8">
         <v>130.27799999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S8">
+        <v>131.91300000000001</v>
+      </c>
+      <c r="T8">
+        <f t="shared" ref="T8:T18" si="2">S8-R8</f>
+        <v>1.6350000000000193</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="G9">
         <v>-0.105</v>
       </c>
@@ -5114,17 +5344,31 @@
         <f t="shared" si="0"/>
         <v>32.971000000000004</v>
       </c>
-      <c r="L9">
+      <c r="J9">
+        <v>263.88299999999998</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>2.9119999999999777</v>
+      </c>
+      <c r="P9">
         <v>1</v>
       </c>
-      <c r="M9">
+      <c r="Q9">
         <v>1.2010000000000001</v>
       </c>
-      <c r="N9">
+      <c r="R9">
         <v>129.38499999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S9">
+        <v>130.53299999999999</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="2"/>
+        <v>1.1479999999999961</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="G10">
         <v>-4.0000000000000001E-3</v>
       </c>
@@ -5135,17 +5379,31 @@
         <f t="shared" si="0"/>
         <v>35.882999999999981</v>
       </c>
-      <c r="L10">
+      <c r="J10">
+        <v>266.33</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>2.4470000000000027</v>
+      </c>
+      <c r="P10">
         <v>2</v>
       </c>
-      <c r="M10">
+      <c r="Q10">
         <v>1.83</v>
       </c>
-      <c r="N10">
+      <c r="R10">
         <v>123.929</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S10">
+        <v>127.47499999999999</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="2"/>
+        <v>3.5459999999999923</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="G11">
         <v>-4.0000000000000001E-3</v>
       </c>
@@ -5156,17 +5414,31 @@
         <f t="shared" si="0"/>
         <v>40.077999999999975</v>
       </c>
-      <c r="L11">
+      <c r="J11">
+        <v>270.75700000000001</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>2.6790000000000305</v>
+      </c>
+      <c r="P11">
         <v>2</v>
       </c>
-      <c r="M11">
+      <c r="Q11">
         <v>2.0840000000000001</v>
       </c>
-      <c r="N11">
+      <c r="R11">
         <v>127.996</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S11">
+        <v>128.95500000000001</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="2"/>
+        <v>0.95900000000001739</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="G12">
         <v>0.58699999999999997</v>
       </c>
@@ -5177,17 +5449,31 @@
         <f t="shared" si="0"/>
         <v>41.009999999999991</v>
       </c>
-      <c r="L12">
+      <c r="J12">
+        <v>276</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>6.9900000000000091</v>
+      </c>
+      <c r="P12">
         <v>2</v>
       </c>
-      <c r="M12">
+      <c r="Q12">
         <v>2.2360000000000002</v>
       </c>
-      <c r="N12">
+      <c r="R12">
         <v>127.004</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S12">
+        <v>128.95500000000001</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="2"/>
+        <v>1.9510000000000076</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="G13">
         <v>0.68799999999999994</v>
       </c>
@@ -5198,17 +5484,31 @@
         <f t="shared" si="0"/>
         <v>45.086999999999989</v>
       </c>
-      <c r="L13">
+      <c r="J13">
+        <v>274.83499999999998</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>1.7479999999999905</v>
+      </c>
+      <c r="P13">
         <v>3</v>
       </c>
-      <c r="M13">
+      <c r="Q13">
         <v>2.6619999999999999</v>
       </c>
-      <c r="N13">
+      <c r="R13">
         <v>124.821</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S13">
+        <v>128.65899999999999</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="2"/>
+        <v>3.8379999999999939</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="G14">
         <v>1.59</v>
       </c>
@@ -5219,66 +5519,108 @@
         <f t="shared" si="0"/>
         <v>44.038999999999987</v>
       </c>
-      <c r="L14">
+      <c r="J14">
+        <v>275.88299999999998</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999941</v>
+      </c>
+      <c r="P14">
         <v>4</v>
       </c>
-      <c r="M14">
+      <c r="Q14">
         <v>3.6259999999999999</v>
       </c>
-      <c r="N14">
+      <c r="R14">
         <v>121.64700000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="L15">
+      <c r="S14">
+        <v>122.84</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="2"/>
+        <v>1.1929999999999978</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="P15">
         <v>4</v>
       </c>
-      <c r="M15">
+      <c r="Q15">
         <v>3.7480000000000002</v>
       </c>
-      <c r="N15">
+      <c r="R15">
         <v>120.556</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="L16">
+      <c r="S15">
+        <v>126.39100000000001</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="2"/>
+        <v>5.835000000000008</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="P16">
         <v>4</v>
       </c>
-      <c r="M16">
+      <c r="Q16">
         <v>4.0519999999999996</v>
       </c>
-      <c r="N16">
+      <c r="R16">
         <v>115.39700000000001</v>
       </c>
-    </row>
-    <row r="17" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="L17">
+      <c r="S16">
+        <v>120.67100000000001</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="2"/>
+        <v>5.2740000000000009</v>
+      </c>
+    </row>
+    <row r="17" spans="5:20" x14ac:dyDescent="0.2">
+      <c r="P17">
         <v>5</v>
       </c>
-      <c r="M17">
+      <c r="Q17">
         <v>4.8639999999999999</v>
       </c>
-      <c r="N17">
+      <c r="R17">
         <v>108.849</v>
       </c>
-    </row>
-    <row r="18" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="L18">
+      <c r="S17">
+        <v>114.556</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="2"/>
+        <v>5.7069999999999936</v>
+      </c>
+    </row>
+    <row r="18" spans="5:20" x14ac:dyDescent="0.2">
+      <c r="P18">
         <v>5</v>
       </c>
-      <c r="M18">
+      <c r="Q18">
         <v>5.3609999999999998</v>
       </c>
-      <c r="N18">
+      <c r="R18">
         <v>106.76600000000001</v>
       </c>
-    </row>
-    <row r="19" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="S18">
+        <v>113.964</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="2"/>
+        <v>7.1979999999999933</v>
+      </c>
+    </row>
+    <row r="19" spans="5:20" x14ac:dyDescent="0.2">
       <c r="E19" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="20" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="5:20" x14ac:dyDescent="0.2">
       <c r="E20" t="s">
         <v>302</v>
       </c>
@@ -5288,8 +5630,17 @@
       <c r="H20" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="21" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="I20" t="s">
+        <v>321</v>
+      </c>
+      <c r="J20" t="s">
+        <v>322</v>
+      </c>
+      <c r="K20" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="21" spans="5:20" x14ac:dyDescent="0.2">
       <c r="E21" t="s">
         <v>310</v>
       </c>
@@ -5297,119 +5648,832 @@
         <v>311</v>
       </c>
       <c r="G21">
-        <v>-4.0000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="H21">
-        <v>257.94200000000001</v>
+        <v>257.73</v>
       </c>
       <c r="I21">
         <f>H21-173</f>
-        <v>84.942000000000007</v>
-      </c>
-    </row>
-    <row r="22" spans="5:14" x14ac:dyDescent="0.2">
+        <v>84.730000000000018</v>
+      </c>
+      <c r="J21">
+        <v>260.971</v>
+      </c>
+      <c r="K21">
+        <f>J21-H21</f>
+        <v>3.2409999999999854</v>
+      </c>
+    </row>
+    <row r="22" spans="5:20" x14ac:dyDescent="0.2">
       <c r="F22" t="s">
         <v>311</v>
       </c>
       <c r="G22">
-        <v>8.5999999999999993E-2</v>
+        <v>0.105</v>
       </c>
       <c r="H22">
-        <v>257.94200000000001</v>
+        <v>257.73</v>
       </c>
       <c r="I22">
-        <f t="shared" ref="I22:I28" si="1">H22-173</f>
-        <v>84.942000000000007</v>
-      </c>
-    </row>
-    <row r="23" spans="5:14" x14ac:dyDescent="0.2">
+        <f t="shared" ref="I22:I28" si="3">H22-173</f>
+        <v>84.730000000000018</v>
+      </c>
+      <c r="J22">
+        <v>261.90300000000002</v>
+      </c>
+      <c r="K22">
+        <f t="shared" ref="K22:K28" si="4">J22-H22</f>
+        <v>4.1730000000000018</v>
+      </c>
+    </row>
+    <row r="23" spans="5:20" x14ac:dyDescent="0.2">
       <c r="F23">
         <v>1</v>
       </c>
       <c r="G23">
-        <v>0.98899999999999999</v>
+        <v>1.0009999999999999</v>
       </c>
       <c r="H23">
-        <v>264.93200000000002</v>
+        <v>264.892</v>
       </c>
       <c r="I23">
-        <f t="shared" si="1"/>
-        <v>91.932000000000016</v>
-      </c>
-    </row>
-    <row r="24" spans="5:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>91.891999999999996</v>
+      </c>
+      <c r="J23">
+        <v>267.029</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="4"/>
+        <v>2.1370000000000005</v>
+      </c>
+    </row>
+    <row r="24" spans="5:20" x14ac:dyDescent="0.2">
       <c r="F24">
         <v>1</v>
       </c>
       <c r="G24">
-        <v>1.1890000000000001</v>
+        <v>1.2030000000000001</v>
       </c>
       <c r="H24">
-        <v>265.98099999999999</v>
+        <v>265.83199999999999</v>
       </c>
       <c r="I24">
-        <f t="shared" si="1"/>
-        <v>92.980999999999995</v>
-      </c>
-    </row>
-    <row r="25" spans="5:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>92.831999999999994</v>
+      </c>
+      <c r="J24">
+        <v>269.12599999999998</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="4"/>
+        <v>3.2939999999999827</v>
+      </c>
+    </row>
+    <row r="25" spans="5:20" x14ac:dyDescent="0.2">
       <c r="F25">
         <v>1</v>
       </c>
       <c r="G25">
-        <v>1.089</v>
+        <v>1.1020000000000001</v>
       </c>
       <c r="H25">
-        <v>277.04899999999998</v>
+        <v>276.98599999999999</v>
       </c>
       <c r="I25">
-        <f t="shared" si="1"/>
-        <v>104.04899999999998</v>
-      </c>
-    </row>
-    <row r="26" spans="5:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>103.98599999999999</v>
+      </c>
+      <c r="J25">
+        <v>279.14600000000002</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="4"/>
+        <v>2.160000000000025</v>
+      </c>
+    </row>
+    <row r="26" spans="5:20" x14ac:dyDescent="0.2">
       <c r="F26">
         <v>3</v>
       </c>
       <c r="G26">
-        <v>2.4830000000000001</v>
+        <v>2.512</v>
       </c>
       <c r="H26">
-        <v>280.07799999999997</v>
+        <v>280.03899999999999</v>
       </c>
       <c r="I26">
-        <f t="shared" si="1"/>
-        <v>107.07799999999997</v>
-      </c>
-    </row>
-    <row r="27" spans="5:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>107.03899999999999</v>
+      </c>
+      <c r="J26">
+        <v>286.13600000000002</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="4"/>
+        <v>6.0970000000000368</v>
+      </c>
+    </row>
+    <row r="27" spans="5:20" x14ac:dyDescent="0.2">
       <c r="F27">
         <v>3</v>
       </c>
       <c r="G27">
-        <v>2.984</v>
+        <v>3.0059999999999998</v>
       </c>
       <c r="H27">
-        <v>279.96100000000001</v>
+        <v>280.03899999999999</v>
       </c>
       <c r="I27">
-        <f t="shared" si="1"/>
-        <v>106.96100000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="5:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>107.03899999999999</v>
+      </c>
+      <c r="J27">
+        <v>286.13600000000002</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="4"/>
+        <v>6.0970000000000368</v>
+      </c>
+    </row>
+    <row r="28" spans="5:20" x14ac:dyDescent="0.2">
       <c r="F28">
         <v>4</v>
       </c>
       <c r="G28">
-        <v>4.3780000000000001</v>
+        <v>4.4160000000000004</v>
       </c>
       <c r="H28">
-        <v>289.16500000000002</v>
+        <v>289.19799999999998</v>
       </c>
       <c r="I28">
-        <f t="shared" si="1"/>
-        <v>116.16500000000002</v>
+        <f t="shared" si="3"/>
+        <v>116.19799999999998</v>
+      </c>
+      <c r="J28">
+        <v>292.19400000000002</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="4"/>
+        <v>2.9960000000000377</v>
+      </c>
+    </row>
+    <row r="32" spans="5:20" x14ac:dyDescent="0.2">
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <v>20</v>
+      </c>
+      <c r="P32">
+        <v>20</v>
+      </c>
+      <c r="Q32">
+        <v>20</v>
+      </c>
+      <c r="R32">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+      <c r="S32">
+        <v>260.971</v>
+      </c>
+    </row>
+    <row r="33" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="M33">
+        <v>2</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <v>194</v>
+      </c>
+      <c r="P33">
+        <v>194</v>
+      </c>
+      <c r="Q33">
+        <v>194</v>
+      </c>
+      <c r="R33">
+        <v>0.115</v>
+      </c>
+      <c r="S33">
+        <v>261.90300000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="M34">
+        <v>3</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <v>171</v>
+      </c>
+      <c r="P34">
+        <v>171</v>
+      </c>
+      <c r="Q34">
+        <v>171</v>
+      </c>
+      <c r="R34">
+        <v>1.012</v>
+      </c>
+      <c r="S34">
+        <v>267.029</v>
+      </c>
+    </row>
+    <row r="35" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>76</v>
+      </c>
+      <c r="F35">
+        <v>76</v>
+      </c>
+      <c r="G35">
+        <v>76</v>
+      </c>
+      <c r="H35">
+        <v>-1.6990000000000001</v>
+      </c>
+      <c r="I35">
+        <v>255.845</v>
+      </c>
+      <c r="M35">
+        <v>4</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <v>109</v>
+      </c>
+      <c r="P35">
+        <v>109</v>
+      </c>
+      <c r="Q35">
+        <v>109</v>
+      </c>
+      <c r="R35">
+        <v>1.2230000000000001</v>
+      </c>
+      <c r="S35">
+        <v>269.12599999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>94</v>
+      </c>
+      <c r="F36">
+        <v>94</v>
+      </c>
+      <c r="G36">
+        <v>94</v>
+      </c>
+      <c r="H36">
+        <v>-1.4990000000000001</v>
+      </c>
+      <c r="I36">
+        <v>253.864</v>
+      </c>
+      <c r="M36">
+        <v>5</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <v>77</v>
+      </c>
+      <c r="P36">
+        <v>77</v>
+      </c>
+      <c r="Q36">
+        <v>77</v>
+      </c>
+      <c r="R36">
+        <v>1.1020000000000001</v>
+      </c>
+      <c r="S36">
+        <v>279.14600000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>92</v>
+      </c>
+      <c r="F37">
+        <v>92</v>
+      </c>
+      <c r="G37">
+        <v>92</v>
+      </c>
+      <c r="H37">
+        <v>-0.59599999999999997</v>
+      </c>
+      <c r="I37">
+        <v>261.786</v>
+      </c>
+      <c r="M37">
+        <v>6</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <v>71</v>
+      </c>
+      <c r="P37">
+        <v>71</v>
+      </c>
+      <c r="Q37">
+        <v>71</v>
+      </c>
+      <c r="R37">
+        <v>2.512</v>
+      </c>
+      <c r="S37">
+        <v>286.13600000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C38">
+        <v>4</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>93</v>
+      </c>
+      <c r="F38">
+        <v>93</v>
+      </c>
+      <c r="G38">
+        <v>93</v>
+      </c>
+      <c r="H38">
+        <v>-0.115</v>
+      </c>
+      <c r="I38">
+        <v>263.88299999999998</v>
+      </c>
+      <c r="M38">
+        <v>7</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <v>124</v>
+      </c>
+      <c r="P38">
+        <v>124</v>
+      </c>
+      <c r="Q38">
+        <v>124</v>
+      </c>
+      <c r="R38">
+        <v>2.996</v>
+      </c>
+      <c r="S38">
+        <v>286.13600000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C39">
+        <v>5</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>169</v>
+      </c>
+      <c r="F39">
+        <v>169</v>
+      </c>
+      <c r="G39">
+        <v>169</v>
+      </c>
+      <c r="H39">
+        <v>1.6E-2</v>
+      </c>
+      <c r="I39">
+        <v>266.33</v>
+      </c>
+      <c r="M39">
+        <v>8</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <v>92</v>
+      </c>
+      <c r="P39">
+        <v>92</v>
+      </c>
+      <c r="Q39">
+        <v>92</v>
+      </c>
+      <c r="R39">
+        <v>4.4260000000000002</v>
+      </c>
+      <c r="S39">
+        <v>292.19400000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C40">
+        <v>6</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>140</v>
+      </c>
+      <c r="F40">
+        <v>140</v>
+      </c>
+      <c r="G40">
+        <v>140</v>
+      </c>
+      <c r="H40">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="I40">
+        <v>270.75700000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C41">
+        <v>7</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>141</v>
+      </c>
+      <c r="F41">
+        <v>141</v>
+      </c>
+      <c r="G41">
+        <v>141</v>
+      </c>
+      <c r="H41">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="I41">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="42" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C42">
+        <v>8</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>72</v>
+      </c>
+      <c r="F42">
+        <v>72</v>
+      </c>
+      <c r="G42">
+        <v>72</v>
+      </c>
+      <c r="H42">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="I42">
+        <v>274.83499999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C43">
+        <v>9</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>23</v>
+      </c>
+      <c r="F43">
+        <v>23</v>
+      </c>
+      <c r="G43">
+        <v>23</v>
+      </c>
+      <c r="H43">
+        <v>1.6</v>
+      </c>
+      <c r="I43">
+        <v>275.88299999999998</v>
+      </c>
+    </row>
+    <row r="50" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="L50">
+        <v>2</v>
+      </c>
+      <c r="M50">
+        <v>0</v>
+      </c>
+      <c r="N50">
+        <v>94</v>
+      </c>
+      <c r="O50">
+        <v>94</v>
+      </c>
+      <c r="P50">
+        <v>94</v>
+      </c>
+      <c r="Q50">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="R50">
+        <v>135.36500000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="L51">
+        <v>3</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+      <c r="N51">
+        <v>89</v>
+      </c>
+      <c r="O51">
+        <v>89</v>
+      </c>
+      <c r="P51">
+        <v>89</v>
+      </c>
+      <c r="Q51">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="R51">
+        <v>131.91300000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="L52">
+        <v>4</v>
+      </c>
+      <c r="M52">
+        <v>0</v>
+      </c>
+      <c r="N52">
+        <v>100</v>
+      </c>
+      <c r="O52">
+        <v>100</v>
+      </c>
+      <c r="P52">
+        <v>100</v>
+      </c>
+      <c r="Q52">
+        <v>1.1819999999999999</v>
+      </c>
+      <c r="R52">
+        <v>130.53299999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="L53">
+        <v>5</v>
+      </c>
+      <c r="M53">
+        <v>0</v>
+      </c>
+      <c r="N53">
+        <v>153</v>
+      </c>
+      <c r="O53">
+        <v>153</v>
+      </c>
+      <c r="P53">
+        <v>153</v>
+      </c>
+      <c r="Q53">
+        <v>1.8080000000000001</v>
+      </c>
+      <c r="R53">
+        <v>127.47499999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="L54">
+        <v>6</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54">
+        <v>164</v>
+      </c>
+      <c r="O54">
+        <v>164</v>
+      </c>
+      <c r="P54">
+        <v>164</v>
+      </c>
+      <c r="Q54">
+        <v>2.0609999999999999</v>
+      </c>
+      <c r="R54">
+        <v>128.95500000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="L55">
+        <v>7</v>
+      </c>
+      <c r="M55">
+        <v>0</v>
+      </c>
+      <c r="N55">
+        <v>95</v>
+      </c>
+      <c r="O55">
+        <v>95</v>
+      </c>
+      <c r="P55">
+        <v>95</v>
+      </c>
+      <c r="Q55">
+        <v>2.222</v>
+      </c>
+      <c r="R55">
+        <v>128.95500000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="L56">
+        <v>8</v>
+      </c>
+      <c r="M56">
+        <v>0</v>
+      </c>
+      <c r="N56">
+        <v>43</v>
+      </c>
+      <c r="O56">
+        <v>43</v>
+      </c>
+      <c r="P56">
+        <v>43</v>
+      </c>
+      <c r="Q56">
+        <v>2.6459999999999999</v>
+      </c>
+      <c r="R56">
+        <v>128.65899999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="L57">
+        <v>9</v>
+      </c>
+      <c r="M57">
+        <v>0</v>
+      </c>
+      <c r="N57">
+        <v>83</v>
+      </c>
+      <c r="O57">
+        <v>83</v>
+      </c>
+      <c r="P57">
+        <v>83</v>
+      </c>
+      <c r="Q57">
+        <v>3.6059999999999999</v>
+      </c>
+      <c r="R57">
+        <v>122.84</v>
+      </c>
+    </row>
+    <row r="58" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="L58">
+        <v>10</v>
+      </c>
+      <c r="M58">
+        <v>0</v>
+      </c>
+      <c r="N58">
+        <v>122</v>
+      </c>
+      <c r="O58">
+        <v>122</v>
+      </c>
+      <c r="P58">
+        <v>122</v>
+      </c>
+      <c r="Q58">
+        <v>3.7370000000000001</v>
+      </c>
+      <c r="R58">
+        <v>126.39100000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="L59">
+        <v>11</v>
+      </c>
+      <c r="M59">
+        <v>0</v>
+      </c>
+      <c r="N59">
+        <v>119</v>
+      </c>
+      <c r="O59">
+        <v>119</v>
+      </c>
+      <c r="P59">
+        <v>119</v>
+      </c>
+      <c r="Q59">
+        <v>4.03</v>
+      </c>
+      <c r="R59">
+        <v>120.67100000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="L60">
+        <v>12</v>
+      </c>
+      <c r="M60">
+        <v>0</v>
+      </c>
+      <c r="N60">
+        <v>56</v>
+      </c>
+      <c r="O60">
+        <v>56</v>
+      </c>
+      <c r="P60">
+        <v>56</v>
+      </c>
+      <c r="Q60">
+        <v>4.8380000000000001</v>
+      </c>
+      <c r="R60">
+        <v>114.556</v>
+      </c>
+    </row>
+    <row r="61" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="L61">
+        <v>13</v>
+      </c>
+      <c r="M61">
+        <v>0</v>
+      </c>
+      <c r="N61">
+        <v>68</v>
+      </c>
+      <c r="O61">
+        <v>68</v>
+      </c>
+      <c r="P61">
+        <v>68</v>
+      </c>
+      <c r="Q61">
+        <v>5.343</v>
+      </c>
+      <c r="R61">
+        <v>113.964</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated fu18 with Darwin's suggestions
</commit_message>
<xml_diff>
--- a/data/update2019/ospree_2019update_dmb.xlsx
+++ b/data/update2019/ospree_2019update_dmb.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="960" windowWidth="25600" windowHeight="15360" activeTab="3"/>
+    <workbookView xWindow="3200" yWindow="960" windowWidth="25600" windowHeight="15360" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="2" r:id="rId1"/>
@@ -952,9 +952,6 @@
     <t>Fagus sylvatica</t>
   </si>
   <si>
-    <t>ambient,ambient,ambient+1</t>
-  </si>
-  <si>
     <t>senescence</t>
   </si>
   <si>
@@ -1003,9 +1000,6 @@
     <t>yadj</t>
   </si>
   <si>
-    <t>daystoenescence</t>
-  </si>
-  <si>
     <t>fig1b</t>
   </si>
   <si>
@@ -1064,6 +1058,12 @@
   </si>
   <si>
     <t>unspecified</t>
+  </si>
+  <si>
+    <t>daystosenescence</t>
+  </si>
+  <si>
+    <t>ambient-1,ambient,ambient+1</t>
   </si>
 </sst>
 </file>
@@ -2887,9 +2887,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2970,13 +2970,13 @@
         <v>287</v>
       </c>
       <c r="M2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="N2">
         <v>4</v>
       </c>
       <c r="T2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -2990,13 +2990,13 @@
         <v>287</v>
       </c>
       <c r="M3" t="s">
-        <v>288</v>
+        <v>325</v>
       </c>
       <c r="N3">
         <v>3</v>
       </c>
       <c r="T3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
@@ -3010,13 +3010,13 @@
         <v>287</v>
       </c>
       <c r="M4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="N4">
         <v>6</v>
       </c>
       <c r="T4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -3033,8 +3033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2:AC30"/>
+    <sheetView topLeftCell="E1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="AF2" sqref="AF2:AG30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3212,46 +3212,40 @@
         <v>284</v>
       </c>
       <c r="C2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D2" t="s">
         <v>286</v>
       </c>
       <c r="E2" t="s">
+        <v>292</v>
+      </c>
+      <c r="G2" t="s">
         <v>293</v>
       </c>
-      <c r="G2" t="s">
+      <c r="M2" t="s">
         <v>294</v>
-      </c>
-      <c r="J2">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K2">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M2" t="s">
-        <v>295</v>
       </c>
       <c r="N2">
         <v>2016</v>
       </c>
       <c r="O2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q2" s="18">
         <v>42597</v>
       </c>
       <c r="U2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="V2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="Y2" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
       <c r="Z2">
         <v>1</v>
@@ -3263,13 +3257,19 @@
         <v>4</v>
       </c>
       <c r="AC2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD2">
         <v>3.8449999999999989</v>
       </c>
       <c r="AE2" t="s">
-        <v>306</v>
+        <v>304</v>
+      </c>
+      <c r="AF2">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG2">
+        <v>4.3499999999999996</v>
       </c>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.2">
@@ -3280,46 +3280,40 @@
         <v>284</v>
       </c>
       <c r="C3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D3" t="s">
         <v>286</v>
       </c>
       <c r="E3" t="s">
+        <v>292</v>
+      </c>
+      <c r="G3" t="s">
         <v>293</v>
       </c>
-      <c r="G3" t="s">
+      <c r="M3" t="s">
         <v>294</v>
-      </c>
-      <c r="J3">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K3">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M3" t="s">
-        <v>295</v>
       </c>
       <c r="N3">
         <v>2016</v>
       </c>
       <c r="O3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q3" s="18">
         <v>42597</v>
       </c>
       <c r="U3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="V3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="Y3" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
       <c r="Z3">
         <v>1</v>
@@ -3331,13 +3325,19 @@
         <v>4</v>
       </c>
       <c r="AC3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD3">
         <v>3.0289999999999964</v>
       </c>
       <c r="AE3" t="s">
-        <v>306</v>
+        <v>304</v>
+      </c>
+      <c r="AF3">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG3">
+        <v>4.3499999999999996</v>
       </c>
     </row>
     <row r="4" spans="1:53" x14ac:dyDescent="0.2">
@@ -3348,46 +3348,40 @@
         <v>284</v>
       </c>
       <c r="C4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D4" t="s">
         <v>286</v>
       </c>
       <c r="E4" t="s">
+        <v>292</v>
+      </c>
+      <c r="G4" t="s">
         <v>293</v>
       </c>
-      <c r="G4" t="s">
+      <c r="M4" t="s">
         <v>294</v>
-      </c>
-      <c r="J4">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K4">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M4" t="s">
-        <v>295</v>
       </c>
       <c r="N4">
         <v>2016</v>
       </c>
       <c r="O4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q4" s="18">
         <v>42597</v>
       </c>
       <c r="U4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="V4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="Y4" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
       <c r="Z4">
         <v>1</v>
@@ -3399,13 +3393,19 @@
         <v>4</v>
       </c>
       <c r="AC4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD4">
         <v>2.7959999999999923</v>
       </c>
       <c r="AE4" t="s">
-        <v>306</v>
+        <v>304</v>
+      </c>
+      <c r="AF4">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG4">
+        <v>4.3499999999999996</v>
       </c>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.2">
@@ -3416,46 +3416,40 @@
         <v>284</v>
       </c>
       <c r="C5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D5" t="s">
         <v>286</v>
       </c>
       <c r="E5" t="s">
+        <v>292</v>
+      </c>
+      <c r="G5" t="s">
         <v>293</v>
       </c>
-      <c r="G5" t="s">
+      <c r="M5" t="s">
         <v>294</v>
-      </c>
-      <c r="J5">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K5">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M5" t="s">
-        <v>295</v>
       </c>
       <c r="N5">
         <v>2016</v>
       </c>
       <c r="O5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q5" s="18">
         <v>42597</v>
       </c>
       <c r="U5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="V5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="Y5" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
       <c r="Z5">
         <v>1</v>
@@ -3467,13 +3461,19 @@
         <v>4</v>
       </c>
       <c r="AC5" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD5">
         <v>2.9119999999999777</v>
       </c>
       <c r="AE5" t="s">
-        <v>306</v>
+        <v>304</v>
+      </c>
+      <c r="AF5">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG5">
+        <v>4.3499999999999996</v>
       </c>
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.2">
@@ -3484,46 +3484,40 @@
         <v>284</v>
       </c>
       <c r="C6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D6" t="s">
         <v>286</v>
       </c>
       <c r="E6" t="s">
+        <v>292</v>
+      </c>
+      <c r="G6" t="s">
         <v>293</v>
       </c>
-      <c r="G6" t="s">
+      <c r="M6" t="s">
         <v>294</v>
-      </c>
-      <c r="J6">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K6">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M6" t="s">
-        <v>295</v>
       </c>
       <c r="N6">
         <v>2016</v>
       </c>
       <c r="O6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q6" s="18">
         <v>42597</v>
       </c>
       <c r="U6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="V6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="Y6" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
       <c r="Z6">
         <v>1</v>
@@ -3535,13 +3529,19 @@
         <v>4</v>
       </c>
       <c r="AC6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD6">
         <v>2.4470000000000027</v>
       </c>
       <c r="AE6" t="s">
-        <v>306</v>
+        <v>304</v>
+      </c>
+      <c r="AF6">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG6">
+        <v>4.3499999999999996</v>
       </c>
     </row>
     <row r="7" spans="1:53" x14ac:dyDescent="0.2">
@@ -3552,46 +3552,40 @@
         <v>284</v>
       </c>
       <c r="C7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D7" t="s">
         <v>286</v>
       </c>
       <c r="E7" t="s">
+        <v>292</v>
+      </c>
+      <c r="G7" t="s">
         <v>293</v>
       </c>
-      <c r="G7" t="s">
+      <c r="M7" t="s">
         <v>294</v>
-      </c>
-      <c r="J7">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K7">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M7" t="s">
-        <v>295</v>
       </c>
       <c r="N7">
         <v>2016</v>
       </c>
       <c r="O7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q7" s="18">
         <v>42597</v>
       </c>
       <c r="U7" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="V7" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="Y7" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
       <c r="Z7">
         <v>1</v>
@@ -3603,13 +3597,19 @@
         <v>4</v>
       </c>
       <c r="AC7" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD7">
         <v>2.6790000000000305</v>
       </c>
       <c r="AE7" t="s">
-        <v>306</v>
+        <v>304</v>
+      </c>
+      <c r="AF7">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG7">
+        <v>4.3499999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:53" x14ac:dyDescent="0.2">
@@ -3620,46 +3620,40 @@
         <v>284</v>
       </c>
       <c r="C8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D8" t="s">
         <v>286</v>
       </c>
       <c r="E8" t="s">
+        <v>292</v>
+      </c>
+      <c r="G8" t="s">
         <v>293</v>
       </c>
-      <c r="G8" t="s">
+      <c r="M8" t="s">
         <v>294</v>
-      </c>
-      <c r="J8">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K8">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M8" t="s">
-        <v>295</v>
       </c>
       <c r="N8">
         <v>2016</v>
       </c>
       <c r="O8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q8" s="18">
         <v>42597</v>
       </c>
       <c r="U8" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="V8" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="Y8" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
       <c r="Z8">
         <v>1</v>
@@ -3671,13 +3665,19 @@
         <v>4</v>
       </c>
       <c r="AC8" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD8">
         <v>6.9900000000000091</v>
       </c>
       <c r="AE8" t="s">
-        <v>306</v>
+        <v>304</v>
+      </c>
+      <c r="AF8">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG8">
+        <v>4.3499999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.2">
@@ -3688,46 +3688,40 @@
         <v>284</v>
       </c>
       <c r="C9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D9" t="s">
         <v>286</v>
       </c>
       <c r="E9" t="s">
+        <v>292</v>
+      </c>
+      <c r="G9" t="s">
         <v>293</v>
       </c>
-      <c r="G9" t="s">
+      <c r="M9" t="s">
         <v>294</v>
-      </c>
-      <c r="J9">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K9">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M9" t="s">
-        <v>295</v>
       </c>
       <c r="N9">
         <v>2016</v>
       </c>
       <c r="O9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q9" s="18">
         <v>42597</v>
       </c>
       <c r="U9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="V9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="Y9" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
       <c r="Z9">
         <v>1</v>
@@ -3739,13 +3733,19 @@
         <v>4</v>
       </c>
       <c r="AC9" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD9">
         <v>1.7479999999999905</v>
       </c>
       <c r="AE9" t="s">
-        <v>306</v>
+        <v>304</v>
+      </c>
+      <c r="AF9">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG9">
+        <v>4.3499999999999996</v>
       </c>
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.2">
@@ -3756,46 +3756,40 @@
         <v>284</v>
       </c>
       <c r="C10" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D10" t="s">
         <v>286</v>
       </c>
       <c r="E10" t="s">
+        <v>292</v>
+      </c>
+      <c r="G10" t="s">
         <v>293</v>
       </c>
-      <c r="G10" t="s">
+      <c r="M10" t="s">
         <v>294</v>
-      </c>
-      <c r="J10">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K10">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M10" t="s">
-        <v>295</v>
       </c>
       <c r="N10">
         <v>2016</v>
       </c>
       <c r="O10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q10" s="18">
         <v>42597</v>
       </c>
       <c r="U10" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="V10" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="Y10" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
       <c r="Z10">
         <v>1</v>
@@ -3807,13 +3801,19 @@
         <v>4</v>
       </c>
       <c r="AC10" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD10">
         <v>3.8439999999999941</v>
       </c>
       <c r="AE10" t="s">
-        <v>306</v>
+        <v>304</v>
+      </c>
+      <c r="AF10">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG10">
+        <v>4.3499999999999996</v>
       </c>
     </row>
     <row r="11" spans="1:53" x14ac:dyDescent="0.2">
@@ -3824,46 +3824,40 @@
         <v>283</v>
       </c>
       <c r="C11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D11" t="s">
         <v>286</v>
       </c>
       <c r="E11" t="s">
+        <v>292</v>
+      </c>
+      <c r="G11" t="s">
         <v>293</v>
       </c>
-      <c r="G11" t="s">
+      <c r="M11" t="s">
         <v>294</v>
-      </c>
-      <c r="J11">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K11">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M11" t="s">
-        <v>295</v>
       </c>
       <c r="N11">
         <v>2016</v>
       </c>
       <c r="O11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P11" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q11" s="18">
         <v>42542</v>
       </c>
       <c r="U11" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="V11" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="Y11" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
       <c r="Z11">
         <v>1</v>
@@ -3875,13 +3869,19 @@
         <v>4</v>
       </c>
       <c r="AC11" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD11">
         <v>3.2409999999999854</v>
       </c>
       <c r="AE11" t="s">
-        <v>306</v>
+        <v>304</v>
+      </c>
+      <c r="AF11">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG11">
+        <v>4.3499999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:53" x14ac:dyDescent="0.2">
@@ -3892,46 +3892,40 @@
         <v>283</v>
       </c>
       <c r="C12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D12" t="s">
         <v>286</v>
       </c>
       <c r="E12" t="s">
+        <v>292</v>
+      </c>
+      <c r="G12" t="s">
         <v>293</v>
       </c>
-      <c r="G12" t="s">
+      <c r="M12" t="s">
         <v>294</v>
-      </c>
-      <c r="J12">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K12">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M12" t="s">
-        <v>295</v>
       </c>
       <c r="N12">
         <v>2016</v>
       </c>
       <c r="O12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P12" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q12" s="18">
         <v>42542</v>
       </c>
       <c r="U12" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="V12" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="Y12" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
       <c r="Z12">
         <v>1</v>
@@ -3943,13 +3937,19 @@
         <v>4</v>
       </c>
       <c r="AC12" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD12">
         <v>4.1730000000000018</v>
       </c>
       <c r="AE12" t="s">
-        <v>306</v>
+        <v>304</v>
+      </c>
+      <c r="AF12">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG12">
+        <v>4.3499999999999996</v>
       </c>
     </row>
     <row r="13" spans="1:53" x14ac:dyDescent="0.2">
@@ -3960,46 +3960,40 @@
         <v>283</v>
       </c>
       <c r="C13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D13" t="s">
         <v>286</v>
       </c>
       <c r="E13" t="s">
+        <v>292</v>
+      </c>
+      <c r="G13" t="s">
         <v>293</v>
       </c>
-      <c r="G13" t="s">
+      <c r="M13" t="s">
         <v>294</v>
-      </c>
-      <c r="J13">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K13">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M13" t="s">
-        <v>295</v>
       </c>
       <c r="N13">
         <v>2016</v>
       </c>
       <c r="O13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q13" s="18">
         <v>42542</v>
       </c>
       <c r="U13" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="V13" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="Y13" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
       <c r="Z13">
         <v>1</v>
@@ -4011,13 +4005,19 @@
         <v>4</v>
       </c>
       <c r="AC13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD13">
         <v>2.1370000000000005</v>
       </c>
       <c r="AE13" t="s">
-        <v>306</v>
+        <v>304</v>
+      </c>
+      <c r="AF13">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG13">
+        <v>4.3499999999999996</v>
       </c>
     </row>
     <row r="14" spans="1:53" x14ac:dyDescent="0.2">
@@ -4028,46 +4028,40 @@
         <v>283</v>
       </c>
       <c r="C14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D14" t="s">
         <v>286</v>
       </c>
       <c r="E14" t="s">
+        <v>292</v>
+      </c>
+      <c r="G14" t="s">
         <v>293</v>
       </c>
-      <c r="G14" t="s">
+      <c r="M14" t="s">
         <v>294</v>
-      </c>
-      <c r="J14">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K14">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M14" t="s">
-        <v>295</v>
       </c>
       <c r="N14">
         <v>2016</v>
       </c>
       <c r="O14" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q14" s="18">
         <v>42542</v>
       </c>
       <c r="U14" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="V14" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="Y14" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
       <c r="Z14">
         <v>1</v>
@@ -4079,13 +4073,19 @@
         <v>4</v>
       </c>
       <c r="AC14" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD14">
         <v>3.2939999999999827</v>
       </c>
       <c r="AE14" t="s">
-        <v>306</v>
+        <v>304</v>
+      </c>
+      <c r="AF14">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG14">
+        <v>4.3499999999999996</v>
       </c>
     </row>
     <row r="15" spans="1:53" x14ac:dyDescent="0.2">
@@ -4096,46 +4096,40 @@
         <v>283</v>
       </c>
       <c r="C15" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D15" t="s">
         <v>286</v>
       </c>
       <c r="E15" t="s">
+        <v>292</v>
+      </c>
+      <c r="G15" t="s">
         <v>293</v>
       </c>
-      <c r="G15" t="s">
+      <c r="M15" t="s">
         <v>294</v>
-      </c>
-      <c r="J15">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K15">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M15" t="s">
-        <v>295</v>
       </c>
       <c r="N15">
         <v>2016</v>
       </c>
       <c r="O15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q15" s="18">
         <v>42542</v>
       </c>
       <c r="U15" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="V15" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="Y15" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
       <c r="Z15">
         <v>1</v>
@@ -4147,13 +4141,19 @@
         <v>4</v>
       </c>
       <c r="AC15" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD15">
         <v>2.160000000000025</v>
       </c>
       <c r="AE15" t="s">
-        <v>306</v>
+        <v>304</v>
+      </c>
+      <c r="AF15">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG15">
+        <v>4.3499999999999996</v>
       </c>
     </row>
     <row r="16" spans="1:53" x14ac:dyDescent="0.2">
@@ -4164,46 +4164,40 @@
         <v>283</v>
       </c>
       <c r="C16" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D16" t="s">
         <v>286</v>
       </c>
       <c r="E16" t="s">
+        <v>292</v>
+      </c>
+      <c r="G16" t="s">
         <v>293</v>
       </c>
-      <c r="G16" t="s">
+      <c r="M16" t="s">
         <v>294</v>
-      </c>
-      <c r="J16">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K16">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M16" t="s">
-        <v>295</v>
       </c>
       <c r="N16">
         <v>2016</v>
       </c>
       <c r="O16" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P16" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q16" s="18">
         <v>42542</v>
       </c>
       <c r="U16" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="V16" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="Y16" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
       <c r="Z16">
         <v>1</v>
@@ -4215,16 +4209,22 @@
         <v>4</v>
       </c>
       <c r="AC16" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD16">
         <v>6.0970000000000368</v>
       </c>
       <c r="AE16" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
+        <v>304</v>
+      </c>
+      <c r="AF16">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG16">
+        <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>282</v>
       </c>
@@ -4232,46 +4232,40 @@
         <v>283</v>
       </c>
       <c r="C17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D17" t="s">
         <v>286</v>
       </c>
       <c r="E17" t="s">
+        <v>292</v>
+      </c>
+      <c r="G17" t="s">
         <v>293</v>
       </c>
-      <c r="G17" t="s">
+      <c r="M17" t="s">
         <v>294</v>
-      </c>
-      <c r="J17">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K17">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M17" t="s">
-        <v>295</v>
       </c>
       <c r="N17">
         <v>2016</v>
       </c>
       <c r="O17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q17" s="18">
         <v>42542</v>
       </c>
       <c r="U17" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="V17" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="Y17" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
       <c r="Z17">
         <v>1</v>
@@ -4283,16 +4277,22 @@
         <v>4</v>
       </c>
       <c r="AC17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD17">
         <v>6.0970000000000368</v>
       </c>
       <c r="AE17" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
+        <v>304</v>
+      </c>
+      <c r="AF17">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG17">
+        <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>282</v>
       </c>
@@ -4300,46 +4300,40 @@
         <v>283</v>
       </c>
       <c r="C18" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D18" t="s">
         <v>286</v>
       </c>
       <c r="E18" t="s">
+        <v>292</v>
+      </c>
+      <c r="G18" t="s">
         <v>293</v>
       </c>
-      <c r="G18" t="s">
+      <c r="M18" t="s">
         <v>294</v>
-      </c>
-      <c r="J18">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K18">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M18" t="s">
-        <v>295</v>
       </c>
       <c r="N18">
         <v>2016</v>
       </c>
       <c r="O18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P18" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q18" s="18">
         <v>42542</v>
       </c>
       <c r="U18" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="V18" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="Y18" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
       <c r="Z18">
         <v>1</v>
@@ -4351,16 +4345,22 @@
         <v>4</v>
       </c>
       <c r="AC18" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD18">
         <v>2.9960000000000377</v>
       </c>
       <c r="AE18" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
+        <v>304</v>
+      </c>
+      <c r="AF18">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG18">
+        <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>282</v>
       </c>
@@ -4368,46 +4368,40 @@
         <v>285</v>
       </c>
       <c r="C19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D19" t="s">
         <v>286</v>
       </c>
       <c r="E19" t="s">
+        <v>292</v>
+      </c>
+      <c r="G19" t="s">
         <v>293</v>
       </c>
-      <c r="G19" t="s">
+      <c r="M19" t="s">
         <v>294</v>
-      </c>
-      <c r="J19">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K19">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M19" t="s">
-        <v>295</v>
       </c>
       <c r="N19">
         <v>2016</v>
       </c>
       <c r="O19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P19" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q19" s="18">
         <v>42370</v>
       </c>
       <c r="U19" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="V19" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="Y19" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="Z19">
         <v>1</v>
@@ -4419,16 +4413,22 @@
         <v>4</v>
       </c>
       <c r="AC19" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD19">
         <v>4.3930000000000007</v>
       </c>
       <c r="AE19" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
+        <v>312</v>
+      </c>
+      <c r="AF19">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG19">
+        <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>282</v>
       </c>
@@ -4436,46 +4436,40 @@
         <v>285</v>
       </c>
       <c r="C20" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D20" t="s">
         <v>286</v>
       </c>
       <c r="E20" t="s">
+        <v>292</v>
+      </c>
+      <c r="G20" t="s">
         <v>293</v>
       </c>
-      <c r="G20" t="s">
+      <c r="M20" t="s">
         <v>294</v>
-      </c>
-      <c r="J20">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K20">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M20" t="s">
-        <v>295</v>
       </c>
       <c r="N20">
         <v>2016</v>
       </c>
       <c r="O20" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P20" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q20" s="18">
         <v>42370</v>
       </c>
       <c r="U20" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="V20" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="Y20" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="Z20">
         <v>1</v>
@@ -4487,16 +4481,22 @@
         <v>4</v>
       </c>
       <c r="AC20" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD20">
         <v>1.6350000000000193</v>
       </c>
       <c r="AE20" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
+        <v>312</v>
+      </c>
+      <c r="AF20">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG20">
+        <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>282</v>
       </c>
@@ -4504,46 +4504,40 @@
         <v>285</v>
       </c>
       <c r="C21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D21" t="s">
         <v>286</v>
       </c>
       <c r="E21" t="s">
+        <v>292</v>
+      </c>
+      <c r="G21" t="s">
         <v>293</v>
       </c>
-      <c r="G21" t="s">
+      <c r="M21" t="s">
         <v>294</v>
-      </c>
-      <c r="J21">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K21">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M21" t="s">
-        <v>295</v>
       </c>
       <c r="N21">
         <v>2016</v>
       </c>
       <c r="O21" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P21" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q21" s="18">
         <v>42370</v>
       </c>
       <c r="U21" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="V21" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="Y21" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="Z21">
         <v>1</v>
@@ -4555,16 +4549,22 @@
         <v>4</v>
       </c>
       <c r="AC21" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD21">
         <v>1.1479999999999961</v>
       </c>
       <c r="AE21" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
+        <v>312</v>
+      </c>
+      <c r="AF21">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG21">
+        <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>282</v>
       </c>
@@ -4572,46 +4572,40 @@
         <v>285</v>
       </c>
       <c r="C22" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D22" t="s">
         <v>286</v>
       </c>
       <c r="E22" t="s">
+        <v>292</v>
+      </c>
+      <c r="G22" t="s">
         <v>293</v>
       </c>
-      <c r="G22" t="s">
+      <c r="M22" t="s">
         <v>294</v>
-      </c>
-      <c r="J22">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K22">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M22" t="s">
-        <v>295</v>
       </c>
       <c r="N22">
         <v>2016</v>
       </c>
       <c r="O22" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P22" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q22" s="18">
         <v>42370</v>
       </c>
       <c r="U22" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="V22" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="Y22" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="Z22">
         <v>1</v>
@@ -4623,16 +4617,22 @@
         <v>4</v>
       </c>
       <c r="AC22" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD22">
         <v>3.5459999999999923</v>
       </c>
       <c r="AE22" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
+        <v>312</v>
+      </c>
+      <c r="AF22">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG22">
+        <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>282</v>
       </c>
@@ -4640,46 +4640,40 @@
         <v>285</v>
       </c>
       <c r="C23" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D23" t="s">
         <v>286</v>
       </c>
       <c r="E23" t="s">
+        <v>292</v>
+      </c>
+      <c r="G23" t="s">
         <v>293</v>
       </c>
-      <c r="G23" t="s">
+      <c r="M23" t="s">
         <v>294</v>
-      </c>
-      <c r="J23">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K23">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M23" t="s">
-        <v>295</v>
       </c>
       <c r="N23">
         <v>2016</v>
       </c>
       <c r="O23" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P23" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q23" s="18">
         <v>42370</v>
       </c>
       <c r="U23" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="V23" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="Y23" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="Z23">
         <v>1</v>
@@ -4691,16 +4685,22 @@
         <v>4</v>
       </c>
       <c r="AC23" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD23">
         <v>0.95900000000001739</v>
       </c>
       <c r="AE23" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
+        <v>312</v>
+      </c>
+      <c r="AF23">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG23">
+        <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>282</v>
       </c>
@@ -4708,46 +4708,40 @@
         <v>285</v>
       </c>
       <c r="C24" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D24" t="s">
         <v>286</v>
       </c>
       <c r="E24" t="s">
+        <v>292</v>
+      </c>
+      <c r="G24" t="s">
         <v>293</v>
       </c>
-      <c r="G24" t="s">
+      <c r="M24" t="s">
         <v>294</v>
-      </c>
-      <c r="J24">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K24">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M24" t="s">
-        <v>295</v>
       </c>
       <c r="N24">
         <v>2016</v>
       </c>
       <c r="O24" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P24" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q24" s="18">
         <v>42370</v>
       </c>
       <c r="U24" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="V24" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="Y24" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="Z24">
         <v>1</v>
@@ -4759,16 +4753,22 @@
         <v>4</v>
       </c>
       <c r="AC24" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD24">
         <v>1.9510000000000076</v>
       </c>
       <c r="AE24" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
+        <v>312</v>
+      </c>
+      <c r="AF24">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG24">
+        <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>282</v>
       </c>
@@ -4776,46 +4776,40 @@
         <v>285</v>
       </c>
       <c r="C25" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D25" t="s">
         <v>286</v>
       </c>
       <c r="E25" t="s">
+        <v>292</v>
+      </c>
+      <c r="G25" t="s">
         <v>293</v>
       </c>
-      <c r="G25" t="s">
+      <c r="M25" t="s">
         <v>294</v>
-      </c>
-      <c r="J25">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K25">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M25" t="s">
-        <v>295</v>
       </c>
       <c r="N25">
         <v>2016</v>
       </c>
       <c r="O25" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P25" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q25" s="18">
         <v>42370</v>
       </c>
       <c r="U25" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="V25" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="Y25" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="Z25">
         <v>1</v>
@@ -4827,16 +4821,22 @@
         <v>4</v>
       </c>
       <c r="AC25" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD25">
         <v>3.8379999999999939</v>
       </c>
       <c r="AE25" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
+        <v>312</v>
+      </c>
+      <c r="AF25">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG25">
+        <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>282</v>
       </c>
@@ -4844,46 +4844,40 @@
         <v>285</v>
       </c>
       <c r="C26" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D26" t="s">
         <v>286</v>
       </c>
       <c r="E26" t="s">
+        <v>292</v>
+      </c>
+      <c r="G26" t="s">
         <v>293</v>
       </c>
-      <c r="G26" t="s">
+      <c r="M26" t="s">
         <v>294</v>
-      </c>
-      <c r="J26">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K26">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M26" t="s">
-        <v>295</v>
       </c>
       <c r="N26">
         <v>2016</v>
       </c>
       <c r="O26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P26" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q26" s="18">
         <v>42370</v>
       </c>
       <c r="U26" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="V26" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="Y26" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="Z26">
         <v>1</v>
@@ -4895,16 +4889,22 @@
         <v>4</v>
       </c>
       <c r="AC26" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD26">
         <v>1.1929999999999978</v>
       </c>
       <c r="AE26" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
+        <v>312</v>
+      </c>
+      <c r="AF26">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG26">
+        <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>282</v>
       </c>
@@ -4912,46 +4912,40 @@
         <v>285</v>
       </c>
       <c r="C27" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D27" t="s">
         <v>286</v>
       </c>
       <c r="E27" t="s">
+        <v>292</v>
+      </c>
+      <c r="G27" t="s">
         <v>293</v>
       </c>
-      <c r="G27" t="s">
+      <c r="M27" t="s">
         <v>294</v>
-      </c>
-      <c r="J27">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K27">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M27" t="s">
-        <v>295</v>
       </c>
       <c r="N27">
         <v>2016</v>
       </c>
       <c r="O27" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P27" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q27" s="18">
         <v>42370</v>
       </c>
       <c r="U27" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="V27" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="Y27" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="Z27">
         <v>1</v>
@@ -4963,16 +4957,22 @@
         <v>4</v>
       </c>
       <c r="AC27" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD27">
         <v>5.835000000000008</v>
       </c>
       <c r="AE27" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
+        <v>312</v>
+      </c>
+      <c r="AF27">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG27">
+        <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>282</v>
       </c>
@@ -4980,46 +4980,40 @@
         <v>285</v>
       </c>
       <c r="C28" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D28" t="s">
         <v>286</v>
       </c>
       <c r="E28" t="s">
+        <v>292</v>
+      </c>
+      <c r="G28" t="s">
         <v>293</v>
       </c>
-      <c r="G28" t="s">
+      <c r="M28" t="s">
         <v>294</v>
-      </c>
-      <c r="J28">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K28">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M28" t="s">
-        <v>295</v>
       </c>
       <c r="N28">
         <v>2016</v>
       </c>
       <c r="O28" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P28" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q28" s="18">
         <v>42370</v>
       </c>
       <c r="U28" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="V28" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="Y28" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="Z28">
         <v>1</v>
@@ -5031,16 +5025,22 @@
         <v>4</v>
       </c>
       <c r="AC28" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD28">
         <v>5.2740000000000009</v>
       </c>
       <c r="AE28" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
+        <v>312</v>
+      </c>
+      <c r="AF28">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG28">
+        <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>282</v>
       </c>
@@ -5048,46 +5048,40 @@
         <v>285</v>
       </c>
       <c r="C29" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D29" t="s">
         <v>286</v>
       </c>
       <c r="E29" t="s">
+        <v>292</v>
+      </c>
+      <c r="G29" t="s">
         <v>293</v>
       </c>
-      <c r="G29" t="s">
+      <c r="M29" t="s">
         <v>294</v>
-      </c>
-      <c r="J29">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K29">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M29" t="s">
-        <v>295</v>
       </c>
       <c r="N29">
         <v>2016</v>
       </c>
       <c r="O29" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P29" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q29" s="18">
         <v>42370</v>
       </c>
       <c r="U29" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="V29" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="Y29" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="Z29">
         <v>1</v>
@@ -5099,16 +5093,22 @@
         <v>4</v>
       </c>
       <c r="AC29" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD29">
         <v>5.7069999999999936</v>
       </c>
       <c r="AE29" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
+        <v>312</v>
+      </c>
+      <c r="AF29">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG29">
+        <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>282</v>
       </c>
@@ -5116,46 +5116,40 @@
         <v>285</v>
       </c>
       <c r="C30" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D30" t="s">
         <v>286</v>
       </c>
       <c r="E30" t="s">
+        <v>292</v>
+      </c>
+      <c r="G30" t="s">
         <v>293</v>
       </c>
-      <c r="G30" t="s">
+      <c r="M30" t="s">
         <v>294</v>
-      </c>
-      <c r="J30">
-        <v>51.316666666666599</v>
-      </c>
-      <c r="K30">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="M30" t="s">
-        <v>295</v>
       </c>
       <c r="N30">
         <v>2016</v>
       </c>
       <c r="O30" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P30" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q30" s="18">
         <v>42370</v>
       </c>
       <c r="U30" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="V30" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="Y30" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="Z30">
         <v>1</v>
@@ -5167,13 +5161,19 @@
         <v>4</v>
       </c>
       <c r="AC30" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD30">
         <v>7.1979999999999933</v>
       </c>
       <c r="AE30" t="s">
-        <v>314</v>
+        <v>312</v>
+      </c>
+      <c r="AF30">
+        <v>51.316666666666599</v>
+      </c>
+      <c r="AG30">
+        <v>4.3499999999999996</v>
       </c>
     </row>
   </sheetData>
@@ -5208,27 +5208,27 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G5" t="s">
+        <v>297</v>
+      </c>
+      <c r="H5" t="s">
         <v>298</v>
       </c>
-      <c r="H5" t="s">
-        <v>299</v>
-      </c>
       <c r="I5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J5" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="K5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="E6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G6">
         <v>-1.7090000000000001</v>
@@ -5248,15 +5248,15 @@
         <v>3.8449999999999989</v>
       </c>
       <c r="O6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="P6" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G7">
         <v>-1.5089999999999999</v>
@@ -5276,7 +5276,7 @@
         <v>3.0289999999999964</v>
       </c>
       <c r="O7" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -5314,7 +5314,7 @@
         <v>2.7959999999999923</v>
       </c>
       <c r="O8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -5617,35 +5617,35 @@
     </row>
     <row r="19" spans="5:20" x14ac:dyDescent="0.2">
       <c r="E19" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="20" spans="5:20" x14ac:dyDescent="0.2">
       <c r="E20" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G20" t="s">
+        <v>297</v>
+      </c>
+      <c r="H20" t="s">
         <v>298</v>
       </c>
-      <c r="H20" t="s">
-        <v>299</v>
-      </c>
       <c r="I20" t="s">
+        <v>319</v>
+      </c>
+      <c r="J20" t="s">
+        <v>320</v>
+      </c>
+      <c r="K20" t="s">
         <v>321</v>
-      </c>
-      <c r="J20" t="s">
-        <v>322</v>
-      </c>
-      <c r="K20" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="21" spans="5:20" x14ac:dyDescent="0.2">
       <c r="E21" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F21" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="G21">
         <v>4.0000000000000001E-3</v>
@@ -5667,7 +5667,7 @@
     </row>
     <row r="22" spans="5:20" x14ac:dyDescent="0.2">
       <c r="F22" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="G22">
         <v>0.105</v>

</xml_diff>